<commit_message>
add train special label
</commit_message>
<xml_diff>
--- a/record_mxq.xlsx
+++ b/record_mxq.xlsx
@@ -9,13 +9,14 @@
   </bookViews>
   <sheets>
     <sheet name="record" sheetId="1" r:id="rId1"/>
+    <sheet name="实验" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="85">
   <si>
     <t>Model</t>
   </si>
@@ -98,6 +99,9 @@
     <t>sparsity</t>
   </si>
   <si>
+    <t>l1_decay</t>
+  </si>
+  <si>
     <t>optimizer</t>
   </si>
   <si>
@@ -243,6 +247,30 @@
   </si>
   <si>
     <t>早停有效</t>
+  </si>
+  <si>
+    <t>log-2019-12-17T08-48-17</t>
+  </si>
+  <si>
+    <t>在大数据集上使用sparsity效果不明显</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>combine_delete_repeat，efficientnet-b5</t>
+  </si>
+  <si>
+    <t>MXQ</t>
+  </si>
+  <si>
+    <t>combine_delete_repeat，同时使用cut_mix和sparsity</t>
+  </si>
+  <si>
+    <t>Online</t>
+  </si>
+  <si>
+    <t>combine_expand，增大cut_mix的概率</t>
   </si>
 </sst>
 </file>
@@ -250,10 +278,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -296,6 +324,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -303,14 +339,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,19 +352,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -349,7 +368,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -357,7 +376,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,6 +404,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -377,8 +426,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -393,22 +443,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -422,8 +464,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -432,21 +475,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,7 +573,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,7 +609,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,19 +633,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,31 +705,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,85 +729,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -892,8 +920,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -913,11 +956,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -933,17 +982,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -962,158 +1005,143 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="40" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="42" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="39" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1247,46 +1275,46 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1679,10 +1707,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AMM29"/>
+  <dimension ref="A1:AMN30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="L5" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1700,19 +1728,19 @@
     <col min="12" max="12" width="9" style="5" customWidth="1"/>
     <col min="13" max="13" width="18.3416666666667" style="5" customWidth="1"/>
     <col min="14" max="14" width="14.6333333333333" style="5" customWidth="1"/>
-    <col min="15" max="16" width="16" style="5" customWidth="1"/>
-    <col min="17" max="17" width="12.7" style="5" customWidth="1"/>
-    <col min="18" max="19" width="18.1166666666667" style="5" customWidth="1"/>
-    <col min="20" max="20" width="27.8833333333333" style="5" customWidth="1"/>
-    <col min="21" max="21" width="12.3833333333333" style="5" customWidth="1"/>
-    <col min="22" max="22" width="10.9916666666667" style="5" customWidth="1"/>
-    <col min="23" max="23" width="23.75" style="5" customWidth="1"/>
-    <col min="24" max="24" width="35.9333333333333" style="5" customWidth="1"/>
-    <col min="25" max="25" width="19.4083333333333" style="5" customWidth="1"/>
-    <col min="26" max="1027" width="9" style="5" customWidth="1"/>
+    <col min="15" max="17" width="16" style="5" customWidth="1"/>
+    <col min="18" max="18" width="12.7" style="5" customWidth="1"/>
+    <col min="19" max="20" width="18.1166666666667" style="5" customWidth="1"/>
+    <col min="21" max="21" width="27.8833333333333" style="5" customWidth="1"/>
+    <col min="22" max="22" width="12.3833333333333" style="5" customWidth="1"/>
+    <col min="23" max="23" width="10.9916666666667" style="5" customWidth="1"/>
+    <col min="24" max="24" width="23.75" style="5" customWidth="1"/>
+    <col min="25" max="25" width="35.9333333333333" style="5" customWidth="1"/>
+    <col min="26" max="26" width="19.4083333333333" style="5" customWidth="1"/>
+    <col min="27" max="1028" width="9" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="22.5" customHeight="1" spans="1:25">
+    <row r="1" s="1" customFormat="1" ht="22.5" customHeight="1" spans="1:26">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1738,30 +1766,31 @@
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="29"/>
+      <c r="S1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="S1" s="39"/>
-      <c r="T1" s="40" t="s">
+      <c r="T1" s="39"/>
+      <c r="U1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="V1" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="41" t="s">
+      <c r="W1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="42" t="s">
+      <c r="X1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="X1" s="43" t="s">
+      <c r="Y1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="55" t="s">
+      <c r="Z1" s="52" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" s="2" customFormat="1" ht="22.5" customHeight="1" spans="1:22">
+    <row r="2" s="2" customFormat="1" ht="22.5" customHeight="1" spans="1:23">
       <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
@@ -1819,19 +1848,22 @@
       <c r="S2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="8"/>
+      <c r="T2" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
     </row>
-    <row r="3" ht="22.5" customHeight="1" spans="1:23">
+    <row r="3" ht="22.5" customHeight="1" spans="1:24">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" s="9">
         <v>0.5</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="9">
         <v>256</v>
@@ -1850,7 +1882,7 @@
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K3" s="9">
         <v>24</v>
@@ -1862,41 +1894,42 @@
         <v>0.01</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O3" s="31">
         <v>0.0005</v>
       </c>
       <c r="P3" s="31"/>
-      <c r="Q3" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q3" s="31"/>
       <c r="R3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="9">
+      <c r="S3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T3" s="9">
         <v>1</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="U3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="V3" s="9">
+      <c r="V3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" s="9">
         <v>0.954</v>
       </c>
-      <c r="W3" s="44"/>
+      <c r="X3" s="43"/>
     </row>
-    <row r="4" ht="22.5" customHeight="1" spans="1:23">
+    <row r="4" ht="22.5" customHeight="1" spans="1:24">
       <c r="A4" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" s="9">
         <v>256</v>
@@ -1915,7 +1948,7 @@
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K4" s="9">
         <v>24</v>
@@ -1927,41 +1960,42 @@
         <v>0.01</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O4" s="31">
         <v>0.0005</v>
       </c>
       <c r="P4" s="31"/>
-      <c r="Q4" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q4" s="31"/>
       <c r="R4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S4" s="9">
+      <c r="S4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" s="9">
         <v>1</v>
       </c>
-      <c r="T4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="9">
+      <c r="U4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="V4" s="9">
         <v>0.957</v>
       </c>
-      <c r="V4" s="9">
+      <c r="W4" s="9">
         <v>0.946</v>
       </c>
-      <c r="W4" s="44"/>
+      <c r="X4" s="43"/>
     </row>
-    <row r="5" ht="21.75" customHeight="1" spans="1:23">
+    <row r="5" ht="21.75" customHeight="1" spans="1:24">
       <c r="A5" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B5" s="9">
         <v>0</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D5" s="9">
         <v>256</v>
@@ -1980,7 +2014,7 @@
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K5" s="9">
         <v>24</v>
@@ -1992,41 +2026,42 @@
         <v>0.01</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O5" s="31">
         <v>0.0005</v>
       </c>
       <c r="P5" s="31"/>
-      <c r="Q5" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q5" s="31"/>
       <c r="R5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S5" s="9">
+      <c r="S5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" s="9">
         <v>1</v>
       </c>
-      <c r="T5" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="U5" s="9">
+      <c r="U5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="V5" s="9">
         <v>0.9643</v>
       </c>
-      <c r="V5" s="9">
+      <c r="W5" s="9">
         <v>0.949</v>
       </c>
-      <c r="W5" s="44"/>
+      <c r="X5" s="43"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1" spans="1:23">
+    <row r="6" ht="18.75" customHeight="1" spans="1:24">
       <c r="A6" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="9">
         <v>0</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="9">
         <v>256</v>
@@ -2045,7 +2080,7 @@
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K6" s="9">
         <v>24</v>
@@ -2057,41 +2092,42 @@
         <v>0.01</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O6" s="31">
         <v>0.0005</v>
       </c>
       <c r="P6" s="31"/>
-      <c r="Q6" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q6" s="31"/>
       <c r="R6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" s="9">
         <v>1</v>
       </c>
-      <c r="T6" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U6" s="9">
+      <c r="U6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" s="9">
         <v>0.9669</v>
       </c>
-      <c r="V6" s="9">
+      <c r="W6" s="9">
         <v>0.952</v>
       </c>
-      <c r="W6" s="44"/>
+      <c r="X6" s="43"/>
     </row>
-    <row r="7" ht="18.75" customHeight="1" spans="1:23">
+    <row r="7" ht="18.75" customHeight="1" spans="1:24">
       <c r="A7" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="9">
         <v>0</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" s="9">
         <v>256</v>
@@ -2110,7 +2146,7 @@
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K7" s="9">
         <v>24</v>
@@ -2122,41 +2158,42 @@
         <v>0.01</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O7" s="31">
         <v>0.0005</v>
       </c>
       <c r="P7" s="31"/>
-      <c r="Q7" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q7" s="31"/>
       <c r="R7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S7" s="9">
+      <c r="S7" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" s="9">
         <v>1</v>
-      </c>
-      <c r="T7" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="V7" s="9">
+      <c r="V7" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="W7" s="9">
         <v>0.958</v>
       </c>
-      <c r="W7" s="44"/>
+      <c r="X7" s="43"/>
     </row>
-    <row r="8" ht="19.5" customHeight="1" spans="1:23">
+    <row r="8" ht="19.5" customHeight="1" spans="1:24">
       <c r="A8" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="9">
         <v>0</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="9">
         <v>256</v>
@@ -2175,7 +2212,7 @@
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K8" s="9">
         <v>24</v>
@@ -2187,41 +2224,42 @@
         <v>0.01</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O8" s="31">
         <v>0.0005</v>
       </c>
       <c r="P8" s="31"/>
-      <c r="Q8" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q8" s="31"/>
       <c r="R8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S8" s="9">
+      <c r="S8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T8" s="9">
         <v>1</v>
       </c>
-      <c r="T8" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="U8" s="9">
+      <c r="U8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="V8" s="9">
         <v>0.9663</v>
       </c>
-      <c r="V8" s="9">
+      <c r="W8" s="9">
         <v>0.959</v>
       </c>
-      <c r="W8" s="44"/>
+      <c r="X8" s="43"/>
     </row>
-    <row r="9" ht="17.25" customHeight="1" spans="1:23">
+    <row r="9" ht="17.25" customHeight="1" spans="1:24">
       <c r="A9" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="9">
         <v>0</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="9">
         <v>256</v>
@@ -2240,7 +2278,7 @@
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K9" s="9">
         <v>24</v>
@@ -2252,41 +2290,42 @@
         <v>0.01</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O9" s="31">
         <v>0.0005</v>
       </c>
       <c r="P9" s="31"/>
-      <c r="Q9" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q9" s="31"/>
       <c r="R9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S9" s="9">
+      <c r="S9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T9" s="9">
         <v>1</v>
       </c>
-      <c r="T9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="9">
+      <c r="U9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" s="9">
         <v>0.9673</v>
       </c>
-      <c r="V9" s="9">
+      <c r="W9" s="9">
         <v>0.961</v>
       </c>
-      <c r="W9" s="44"/>
+      <c r="X9" s="43"/>
     </row>
-    <row r="10" ht="17.25" customHeight="1" spans="1:23">
+    <row r="10" ht="17.25" customHeight="1" spans="1:24">
       <c r="A10" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="9">
         <v>0</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="9">
         <v>256</v>
@@ -2305,7 +2344,7 @@
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K10" s="9">
         <v>24</v>
@@ -2317,42 +2356,43 @@
         <v>0.01</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O10" s="31">
         <v>0.0005</v>
       </c>
       <c r="P10" s="31"/>
-      <c r="Q10" s="9" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q10" s="31"/>
       <c r="R10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="S10" s="9">
+      <c r="S10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" s="9">
         <v>0</v>
       </c>
-      <c r="T10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="9">
+      <c r="U10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" s="9">
         <v>0.981</v>
       </c>
-      <c r="V10" s="9">
+      <c r="W10" s="9">
         <v>0.964</v>
       </c>
-      <c r="W10" s="44"/>
+      <c r="X10" s="43"/>
     </row>
     <row r="11" ht="19.5" customHeight="1"/>
-    <row r="12" ht="18" customHeight="1" spans="1:23">
+    <row r="12" ht="18" customHeight="1" spans="1:24">
       <c r="A12" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="10">
         <v>0</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D12" s="10">
         <v>256</v>
@@ -2371,7 +2411,7 @@
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K12" s="9">
         <v>24</v>
@@ -2383,41 +2423,42 @@
         <v>0.002</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O12" s="31">
         <v>0.0005</v>
       </c>
       <c r="P12" s="31"/>
-      <c r="Q12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="R12" s="9" t="s">
+      <c r="Q12" s="31"/>
+      <c r="R12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="S12" s="10">
+      <c r="S12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12" s="10">
         <v>2</v>
       </c>
-      <c r="T12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U12" s="10">
+      <c r="U12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V12" s="10">
         <v>0.9804</v>
       </c>
-      <c r="V12" s="10">
+      <c r="W12" s="10">
         <v>0.964</v>
       </c>
-      <c r="W12" s="44"/>
+      <c r="X12" s="43"/>
     </row>
-    <row r="13" ht="15.75" spans="1:23">
+    <row r="13" spans="1:24">
       <c r="A13" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="10">
         <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D13" s="10">
         <v>256</v>
@@ -2436,7 +2477,7 @@
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K13" s="9">
         <v>24</v>
@@ -2448,41 +2489,42 @@
         <v>0.001</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O13" s="31">
         <v>0.0005</v>
       </c>
       <c r="P13" s="31"/>
-      <c r="Q13" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="R13" s="9" t="s">
+      <c r="Q13" s="31"/>
+      <c r="R13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="S13" s="10">
+      <c r="S13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T13" s="10">
         <v>2</v>
       </c>
-      <c r="T13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U13" s="10">
+      <c r="U13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V13" s="10">
         <v>0.9783</v>
       </c>
-      <c r="V13" s="10">
+      <c r="W13" s="10">
         <v>0.955</v>
       </c>
-      <c r="W13" s="44"/>
+      <c r="X13" s="43"/>
     </row>
-    <row r="14" ht="18" customHeight="1" spans="1:23">
+    <row r="14" ht="18" customHeight="1" spans="1:24">
       <c r="A14" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="10">
         <v>0</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" s="10">
         <v>256</v>
@@ -2501,7 +2543,7 @@
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K14" s="9">
         <v>24</v>
@@ -2510,38 +2552,39 @@
         <v>30</v>
       </c>
       <c r="M14" s="31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O14" s="31">
         <v>0.0005</v>
       </c>
       <c r="P14" s="31"/>
-      <c r="Q14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="R14" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="S14" s="10">
+      <c r="Q14" s="31"/>
+      <c r="R14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="S14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T14" s="10">
         <v>0</v>
       </c>
-      <c r="T14" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U14" s="10">
+      <c r="U14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V14" s="10">
         <v>0.9827</v>
       </c>
-      <c r="V14" s="21">
+      <c r="W14" s="21">
         <v>0.971</v>
       </c>
-      <c r="W14" s="44"/>
+      <c r="X14" s="43"/>
     </row>
-    <row r="15" ht="20.25" customHeight="1" spans="1:22">
+    <row r="15" ht="20.25" customHeight="1" spans="1:23">
       <c r="A15" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -2564,16 +2607,17 @@
       <c r="T15" s="11"/>
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
     </row>
-    <row r="16" ht="18" customHeight="1" spans="1:23">
+    <row r="16" ht="18" customHeight="1" spans="1:24">
       <c r="A16" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="13">
         <v>0</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="13">
         <v>416</v>
@@ -2592,7 +2636,7 @@
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K16" s="12">
         <v>8</v>
@@ -2601,44 +2645,45 @@
         <v>30</v>
       </c>
       <c r="M16" s="32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O16" s="32">
         <v>0.0005</v>
       </c>
       <c r="P16" s="32"/>
-      <c r="Q16" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="R16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="S16" s="13">
+      <c r="Q16" s="32"/>
+      <c r="R16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="T16" s="13">
         <v>0</v>
       </c>
-      <c r="T16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="U16" s="13">
+      <c r="U16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="V16" s="13">
         <v>0.9837</v>
       </c>
-      <c r="V16" s="45">
+      <c r="W16" s="44">
         <v>0.974</v>
       </c>
-      <c r="W16" s="44"/>
+      <c r="X16" s="43"/>
     </row>
-    <row r="17" s="3" customFormat="1" ht="15.75" spans="1:1027">
+    <row r="17" s="3" customFormat="1" ht="15.75" spans="1:1028">
       <c r="A17" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="13">
         <v>0</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D17" s="13">
         <v>256</v>
@@ -2657,7 +2702,7 @@
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K17" s="12">
         <v>24</v>
@@ -2669,1037 +2714,1038 @@
         <v>0.0003</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O17" s="32">
         <v>0.0005</v>
       </c>
       <c r="P17" s="32"/>
-      <c r="Q17" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="R17" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="S17" s="13">
+      <c r="Q17" s="32"/>
+      <c r="R17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="T17" s="13">
         <v>0</v>
       </c>
-      <c r="T17" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="U17" s="13">
+      <c r="U17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="V17" s="13">
         <v>0.9827</v>
       </c>
-      <c r="V17" s="13">
+      <c r="W17" s="13">
         <v>0.955</v>
       </c>
-      <c r="W17" s="46"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="47"/>
-      <c r="Z17" s="47"/>
-      <c r="AA17" s="47"/>
-      <c r="AB17" s="47"/>
-      <c r="AC17" s="47"/>
-      <c r="AD17" s="47"/>
-      <c r="AE17" s="47"/>
-      <c r="AF17" s="47"/>
-      <c r="AG17" s="47"/>
-      <c r="AH17" s="47"/>
-      <c r="AI17" s="47"/>
-      <c r="AJ17" s="47"/>
-      <c r="AK17" s="47"/>
-      <c r="AL17" s="47"/>
-      <c r="AM17" s="47"/>
-      <c r="AN17" s="47"/>
-      <c r="AO17" s="47"/>
-      <c r="AP17" s="47"/>
-      <c r="AQ17" s="47"/>
-      <c r="AR17" s="47"/>
-      <c r="AS17" s="47"/>
-      <c r="AT17" s="47"/>
-      <c r="AU17" s="47"/>
-      <c r="AV17" s="47"/>
-      <c r="AW17" s="47"/>
-      <c r="AX17" s="47"/>
-      <c r="AY17" s="47"/>
-      <c r="AZ17" s="47"/>
-      <c r="BA17" s="47"/>
-      <c r="BB17" s="47"/>
-      <c r="BC17" s="47"/>
-      <c r="BD17" s="47"/>
-      <c r="BE17" s="47"/>
-      <c r="BF17" s="47"/>
-      <c r="BG17" s="47"/>
-      <c r="BH17" s="47"/>
-      <c r="BI17" s="47"/>
-      <c r="BJ17" s="47"/>
-      <c r="BK17" s="47"/>
-      <c r="BL17" s="47"/>
-      <c r="BM17" s="47"/>
-      <c r="BN17" s="47"/>
-      <c r="BO17" s="47"/>
-      <c r="BP17" s="47"/>
-      <c r="BQ17" s="47"/>
-      <c r="BR17" s="47"/>
-      <c r="BS17" s="47"/>
-      <c r="BT17" s="47"/>
-      <c r="BU17" s="47"/>
-      <c r="BV17" s="47"/>
-      <c r="BW17" s="47"/>
-      <c r="BX17" s="47"/>
-      <c r="BY17" s="47"/>
-      <c r="BZ17" s="47"/>
-      <c r="CA17" s="47"/>
-      <c r="CB17" s="47"/>
-      <c r="CC17" s="47"/>
-      <c r="CD17" s="47"/>
-      <c r="CE17" s="47"/>
-      <c r="CF17" s="47"/>
-      <c r="CG17" s="47"/>
-      <c r="CH17" s="47"/>
-      <c r="CI17" s="47"/>
-      <c r="CJ17" s="47"/>
-      <c r="CK17" s="47"/>
-      <c r="CL17" s="47"/>
-      <c r="CM17" s="47"/>
-      <c r="CN17" s="47"/>
-      <c r="CO17" s="47"/>
-      <c r="CP17" s="47"/>
-      <c r="CQ17" s="47"/>
-      <c r="CR17" s="47"/>
-      <c r="CS17" s="47"/>
-      <c r="CT17" s="47"/>
-      <c r="CU17" s="47"/>
-      <c r="CV17" s="47"/>
-      <c r="CW17" s="47"/>
-      <c r="CX17" s="47"/>
-      <c r="CY17" s="47"/>
-      <c r="CZ17" s="47"/>
-      <c r="DA17" s="47"/>
-      <c r="DB17" s="47"/>
-      <c r="DC17" s="47"/>
-      <c r="DD17" s="47"/>
-      <c r="DE17" s="47"/>
-      <c r="DF17" s="47"/>
-      <c r="DG17" s="47"/>
-      <c r="DH17" s="47"/>
-      <c r="DI17" s="47"/>
-      <c r="DJ17" s="47"/>
-      <c r="DK17" s="47"/>
-      <c r="DL17" s="47"/>
-      <c r="DM17" s="47"/>
-      <c r="DN17" s="47"/>
-      <c r="DO17" s="47"/>
-      <c r="DP17" s="47"/>
-      <c r="DQ17" s="47"/>
-      <c r="DR17" s="47"/>
-      <c r="DS17" s="47"/>
-      <c r="DT17" s="47"/>
-      <c r="DU17" s="47"/>
-      <c r="DV17" s="47"/>
-      <c r="DW17" s="47"/>
-      <c r="DX17" s="47"/>
-      <c r="DY17" s="47"/>
-      <c r="DZ17" s="47"/>
-      <c r="EA17" s="47"/>
-      <c r="EB17" s="47"/>
-      <c r="EC17" s="47"/>
-      <c r="ED17" s="47"/>
-      <c r="EE17" s="47"/>
-      <c r="EF17" s="47"/>
-      <c r="EG17" s="47"/>
-      <c r="EH17" s="47"/>
-      <c r="EI17" s="47"/>
-      <c r="EJ17" s="47"/>
-      <c r="EK17" s="47"/>
-      <c r="EL17" s="47"/>
-      <c r="EM17" s="47"/>
-      <c r="EN17" s="47"/>
-      <c r="EO17" s="47"/>
-      <c r="EP17" s="47"/>
-      <c r="EQ17" s="47"/>
-      <c r="ER17" s="47"/>
-      <c r="ES17" s="47"/>
-      <c r="ET17" s="47"/>
-      <c r="EU17" s="47"/>
-      <c r="EV17" s="47"/>
-      <c r="EW17" s="47"/>
-      <c r="EX17" s="47"/>
-      <c r="EY17" s="47"/>
-      <c r="EZ17" s="47"/>
-      <c r="FA17" s="47"/>
-      <c r="FB17" s="47"/>
-      <c r="FC17" s="47"/>
-      <c r="FD17" s="47"/>
-      <c r="FE17" s="47"/>
-      <c r="FF17" s="47"/>
-      <c r="FG17" s="47"/>
-      <c r="FH17" s="47"/>
-      <c r="FI17" s="47"/>
-      <c r="FJ17" s="47"/>
-      <c r="FK17" s="47"/>
-      <c r="FL17" s="47"/>
-      <c r="FM17" s="47"/>
-      <c r="FN17" s="47"/>
-      <c r="FO17" s="47"/>
-      <c r="FP17" s="47"/>
-      <c r="FQ17" s="47"/>
-      <c r="FR17" s="47"/>
-      <c r="FS17" s="47"/>
-      <c r="FT17" s="47"/>
-      <c r="FU17" s="47"/>
-      <c r="FV17" s="47"/>
-      <c r="FW17" s="47"/>
-      <c r="FX17" s="47"/>
-      <c r="FY17" s="47"/>
-      <c r="FZ17" s="47"/>
-      <c r="GA17" s="47"/>
-      <c r="GB17" s="47"/>
-      <c r="GC17" s="47"/>
-      <c r="GD17" s="47"/>
-      <c r="GE17" s="47"/>
-      <c r="GF17" s="47"/>
-      <c r="GG17" s="47"/>
-      <c r="GH17" s="47"/>
-      <c r="GI17" s="47"/>
-      <c r="GJ17" s="47"/>
-      <c r="GK17" s="47"/>
-      <c r="GL17" s="47"/>
-      <c r="GM17" s="47"/>
-      <c r="GN17" s="47"/>
-      <c r="GO17" s="47"/>
-      <c r="GP17" s="47"/>
-      <c r="GQ17" s="47"/>
-      <c r="GR17" s="47"/>
-      <c r="GS17" s="47"/>
-      <c r="GT17" s="47"/>
-      <c r="GU17" s="47"/>
-      <c r="GV17" s="47"/>
-      <c r="GW17" s="47"/>
-      <c r="GX17" s="47"/>
-      <c r="GY17" s="47"/>
-      <c r="GZ17" s="47"/>
-      <c r="HA17" s="47"/>
-      <c r="HB17" s="47"/>
-      <c r="HC17" s="47"/>
-      <c r="HD17" s="47"/>
-      <c r="HE17" s="47"/>
-      <c r="HF17" s="47"/>
-      <c r="HG17" s="47"/>
-      <c r="HH17" s="47"/>
-      <c r="HI17" s="47"/>
-      <c r="HJ17" s="47"/>
-      <c r="HK17" s="47"/>
-      <c r="HL17" s="47"/>
-      <c r="HM17" s="47"/>
-      <c r="HN17" s="47"/>
-      <c r="HO17" s="47"/>
-      <c r="HP17" s="47"/>
-      <c r="HQ17" s="47"/>
-      <c r="HR17" s="47"/>
-      <c r="HS17" s="47"/>
-      <c r="HT17" s="47"/>
-      <c r="HU17" s="47"/>
-      <c r="HV17" s="47"/>
-      <c r="HW17" s="47"/>
-      <c r="HX17" s="47"/>
-      <c r="HY17" s="47"/>
-      <c r="HZ17" s="47"/>
-      <c r="IA17" s="47"/>
-      <c r="IB17" s="47"/>
-      <c r="IC17" s="47"/>
-      <c r="ID17" s="47"/>
-      <c r="IE17" s="47"/>
-      <c r="IF17" s="47"/>
-      <c r="IG17" s="47"/>
-      <c r="IH17" s="47"/>
-      <c r="II17" s="47"/>
-      <c r="IJ17" s="47"/>
-      <c r="IK17" s="47"/>
-      <c r="IL17" s="47"/>
-      <c r="IM17" s="47"/>
-      <c r="IN17" s="47"/>
-      <c r="IO17" s="47"/>
-      <c r="IP17" s="47"/>
-      <c r="IQ17" s="47"/>
-      <c r="IR17" s="47"/>
-      <c r="IS17" s="47"/>
-      <c r="IT17" s="47"/>
-      <c r="IU17" s="47"/>
-      <c r="IV17" s="47"/>
-      <c r="IW17" s="47"/>
-      <c r="IX17" s="47"/>
-      <c r="IY17" s="47"/>
-      <c r="IZ17" s="47"/>
-      <c r="JA17" s="47"/>
-      <c r="JB17" s="47"/>
-      <c r="JC17" s="47"/>
-      <c r="JD17" s="47"/>
-      <c r="JE17" s="47"/>
-      <c r="JF17" s="47"/>
-      <c r="JG17" s="47"/>
-      <c r="JH17" s="47"/>
-      <c r="JI17" s="47"/>
-      <c r="JJ17" s="47"/>
-      <c r="JK17" s="47"/>
-      <c r="JL17" s="47"/>
-      <c r="JM17" s="47"/>
-      <c r="JN17" s="47"/>
-      <c r="JO17" s="47"/>
-      <c r="JP17" s="47"/>
-      <c r="JQ17" s="47"/>
-      <c r="JR17" s="47"/>
-      <c r="JS17" s="47"/>
-      <c r="JT17" s="47"/>
-      <c r="JU17" s="47"/>
-      <c r="JV17" s="47"/>
-      <c r="JW17" s="47"/>
-      <c r="JX17" s="47"/>
-      <c r="JY17" s="47"/>
-      <c r="JZ17" s="47"/>
-      <c r="KA17" s="47"/>
-      <c r="KB17" s="47"/>
-      <c r="KC17" s="47"/>
-      <c r="KD17" s="47"/>
-      <c r="KE17" s="47"/>
-      <c r="KF17" s="47"/>
-      <c r="KG17" s="47"/>
-      <c r="KH17" s="47"/>
-      <c r="KI17" s="47"/>
-      <c r="KJ17" s="47"/>
-      <c r="KK17" s="47"/>
-      <c r="KL17" s="47"/>
-      <c r="KM17" s="47"/>
-      <c r="KN17" s="47"/>
-      <c r="KO17" s="47"/>
-      <c r="KP17" s="47"/>
-      <c r="KQ17" s="47"/>
-      <c r="KR17" s="47"/>
-      <c r="KS17" s="47"/>
-      <c r="KT17" s="47"/>
-      <c r="KU17" s="47"/>
-      <c r="KV17" s="47"/>
-      <c r="KW17" s="47"/>
-      <c r="KX17" s="47"/>
-      <c r="KY17" s="47"/>
-      <c r="KZ17" s="47"/>
-      <c r="LA17" s="47"/>
-      <c r="LB17" s="47"/>
-      <c r="LC17" s="47"/>
-      <c r="LD17" s="47"/>
-      <c r="LE17" s="47"/>
-      <c r="LF17" s="47"/>
-      <c r="LG17" s="47"/>
-      <c r="LH17" s="47"/>
-      <c r="LI17" s="47"/>
-      <c r="LJ17" s="47"/>
-      <c r="LK17" s="47"/>
-      <c r="LL17" s="47"/>
-      <c r="LM17" s="47"/>
-      <c r="LN17" s="47"/>
-      <c r="LO17" s="47"/>
-      <c r="LP17" s="47"/>
-      <c r="LQ17" s="47"/>
-      <c r="LR17" s="47"/>
-      <c r="LS17" s="47"/>
-      <c r="LT17" s="47"/>
-      <c r="LU17" s="47"/>
-      <c r="LV17" s="47"/>
-      <c r="LW17" s="47"/>
-      <c r="LX17" s="47"/>
-      <c r="LY17" s="47"/>
-      <c r="LZ17" s="47"/>
-      <c r="MA17" s="47"/>
-      <c r="MB17" s="47"/>
-      <c r="MC17" s="47"/>
-      <c r="MD17" s="47"/>
-      <c r="ME17" s="47"/>
-      <c r="MF17" s="47"/>
-      <c r="MG17" s="47"/>
-      <c r="MH17" s="47"/>
-      <c r="MI17" s="47"/>
-      <c r="MJ17" s="47"/>
-      <c r="MK17" s="47"/>
-      <c r="ML17" s="47"/>
-      <c r="MM17" s="47"/>
-      <c r="MN17" s="47"/>
-      <c r="MO17" s="47"/>
-      <c r="MP17" s="47"/>
-      <c r="MQ17" s="47"/>
-      <c r="MR17" s="47"/>
-      <c r="MS17" s="47"/>
-      <c r="MT17" s="47"/>
-      <c r="MU17" s="47"/>
-      <c r="MV17" s="47"/>
-      <c r="MW17" s="47"/>
-      <c r="MX17" s="47"/>
-      <c r="MY17" s="47"/>
-      <c r="MZ17" s="47"/>
-      <c r="NA17" s="47"/>
-      <c r="NB17" s="47"/>
-      <c r="NC17" s="47"/>
-      <c r="ND17" s="47"/>
-      <c r="NE17" s="47"/>
-      <c r="NF17" s="47"/>
-      <c r="NG17" s="47"/>
-      <c r="NH17" s="47"/>
-      <c r="NI17" s="47"/>
-      <c r="NJ17" s="47"/>
-      <c r="NK17" s="47"/>
-      <c r="NL17" s="47"/>
-      <c r="NM17" s="47"/>
-      <c r="NN17" s="47"/>
-      <c r="NO17" s="47"/>
-      <c r="NP17" s="47"/>
-      <c r="NQ17" s="47"/>
-      <c r="NR17" s="47"/>
-      <c r="NS17" s="47"/>
-      <c r="NT17" s="47"/>
-      <c r="NU17" s="47"/>
-      <c r="NV17" s="47"/>
-      <c r="NW17" s="47"/>
-      <c r="NX17" s="47"/>
-      <c r="NY17" s="47"/>
-      <c r="NZ17" s="47"/>
-      <c r="OA17" s="47"/>
-      <c r="OB17" s="47"/>
-      <c r="OC17" s="47"/>
-      <c r="OD17" s="47"/>
-      <c r="OE17" s="47"/>
-      <c r="OF17" s="47"/>
-      <c r="OG17" s="47"/>
-      <c r="OH17" s="47"/>
-      <c r="OI17" s="47"/>
-      <c r="OJ17" s="47"/>
-      <c r="OK17" s="47"/>
-      <c r="OL17" s="47"/>
-      <c r="OM17" s="47"/>
-      <c r="ON17" s="47"/>
-      <c r="OO17" s="47"/>
-      <c r="OP17" s="47"/>
-      <c r="OQ17" s="47"/>
-      <c r="OR17" s="47"/>
-      <c r="OS17" s="47"/>
-      <c r="OT17" s="47"/>
-      <c r="OU17" s="47"/>
-      <c r="OV17" s="47"/>
-      <c r="OW17" s="47"/>
-      <c r="OX17" s="47"/>
-      <c r="OY17" s="47"/>
-      <c r="OZ17" s="47"/>
-      <c r="PA17" s="47"/>
-      <c r="PB17" s="47"/>
-      <c r="PC17" s="47"/>
-      <c r="PD17" s="47"/>
-      <c r="PE17" s="47"/>
-      <c r="PF17" s="47"/>
-      <c r="PG17" s="47"/>
-      <c r="PH17" s="47"/>
-      <c r="PI17" s="47"/>
-      <c r="PJ17" s="47"/>
-      <c r="PK17" s="47"/>
-      <c r="PL17" s="47"/>
-      <c r="PM17" s="47"/>
-      <c r="PN17" s="47"/>
-      <c r="PO17" s="47"/>
-      <c r="PP17" s="47"/>
-      <c r="PQ17" s="47"/>
-      <c r="PR17" s="47"/>
-      <c r="PS17" s="47"/>
-      <c r="PT17" s="47"/>
-      <c r="PU17" s="47"/>
-      <c r="PV17" s="47"/>
-      <c r="PW17" s="47"/>
-      <c r="PX17" s="47"/>
-      <c r="PY17" s="47"/>
-      <c r="PZ17" s="47"/>
-      <c r="QA17" s="47"/>
-      <c r="QB17" s="47"/>
-      <c r="QC17" s="47"/>
-      <c r="QD17" s="47"/>
-      <c r="QE17" s="47"/>
-      <c r="QF17" s="47"/>
-      <c r="QG17" s="47"/>
-      <c r="QH17" s="47"/>
-      <c r="QI17" s="47"/>
-      <c r="QJ17" s="47"/>
-      <c r="QK17" s="47"/>
-      <c r="QL17" s="47"/>
-      <c r="QM17" s="47"/>
-      <c r="QN17" s="47"/>
-      <c r="QO17" s="47"/>
-      <c r="QP17" s="47"/>
-      <c r="QQ17" s="47"/>
-      <c r="QR17" s="47"/>
-      <c r="QS17" s="47"/>
-      <c r="QT17" s="47"/>
-      <c r="QU17" s="47"/>
-      <c r="QV17" s="47"/>
-      <c r="QW17" s="47"/>
-      <c r="QX17" s="47"/>
-      <c r="QY17" s="47"/>
-      <c r="QZ17" s="47"/>
-      <c r="RA17" s="47"/>
-      <c r="RB17" s="47"/>
-      <c r="RC17" s="47"/>
-      <c r="RD17" s="47"/>
-      <c r="RE17" s="47"/>
-      <c r="RF17" s="47"/>
-      <c r="RG17" s="47"/>
-      <c r="RH17" s="47"/>
-      <c r="RI17" s="47"/>
-      <c r="RJ17" s="47"/>
-      <c r="RK17" s="47"/>
-      <c r="RL17" s="47"/>
-      <c r="RM17" s="47"/>
-      <c r="RN17" s="47"/>
-      <c r="RO17" s="47"/>
-      <c r="RP17" s="47"/>
-      <c r="RQ17" s="47"/>
-      <c r="RR17" s="47"/>
-      <c r="RS17" s="47"/>
-      <c r="RT17" s="47"/>
-      <c r="RU17" s="47"/>
-      <c r="RV17" s="47"/>
-      <c r="RW17" s="47"/>
-      <c r="RX17" s="47"/>
-      <c r="RY17" s="47"/>
-      <c r="RZ17" s="47"/>
-      <c r="SA17" s="47"/>
-      <c r="SB17" s="47"/>
-      <c r="SC17" s="47"/>
-      <c r="SD17" s="47"/>
-      <c r="SE17" s="47"/>
-      <c r="SF17" s="47"/>
-      <c r="SG17" s="47"/>
-      <c r="SH17" s="47"/>
-      <c r="SI17" s="47"/>
-      <c r="SJ17" s="47"/>
-      <c r="SK17" s="47"/>
-      <c r="SL17" s="47"/>
-      <c r="SM17" s="47"/>
-      <c r="SN17" s="47"/>
-      <c r="SO17" s="47"/>
-      <c r="SP17" s="47"/>
-      <c r="SQ17" s="47"/>
-      <c r="SR17" s="47"/>
-      <c r="SS17" s="47"/>
-      <c r="ST17" s="47"/>
-      <c r="SU17" s="47"/>
-      <c r="SV17" s="47"/>
-      <c r="SW17" s="47"/>
-      <c r="SX17" s="47"/>
-      <c r="SY17" s="47"/>
-      <c r="SZ17" s="47"/>
-      <c r="TA17" s="47"/>
-      <c r="TB17" s="47"/>
-      <c r="TC17" s="47"/>
-      <c r="TD17" s="47"/>
-      <c r="TE17" s="47"/>
-      <c r="TF17" s="47"/>
-      <c r="TG17" s="47"/>
-      <c r="TH17" s="47"/>
-      <c r="TI17" s="47"/>
-      <c r="TJ17" s="47"/>
-      <c r="TK17" s="47"/>
-      <c r="TL17" s="47"/>
-      <c r="TM17" s="47"/>
-      <c r="TN17" s="47"/>
-      <c r="TO17" s="47"/>
-      <c r="TP17" s="47"/>
-      <c r="TQ17" s="47"/>
-      <c r="TR17" s="47"/>
-      <c r="TS17" s="47"/>
-      <c r="TT17" s="47"/>
-      <c r="TU17" s="47"/>
-      <c r="TV17" s="47"/>
-      <c r="TW17" s="47"/>
-      <c r="TX17" s="47"/>
-      <c r="TY17" s="47"/>
-      <c r="TZ17" s="47"/>
-      <c r="UA17" s="47"/>
-      <c r="UB17" s="47"/>
-      <c r="UC17" s="47"/>
-      <c r="UD17" s="47"/>
-      <c r="UE17" s="47"/>
-      <c r="UF17" s="47"/>
-      <c r="UG17" s="47"/>
-      <c r="UH17" s="47"/>
-      <c r="UI17" s="47"/>
-      <c r="UJ17" s="47"/>
-      <c r="UK17" s="47"/>
-      <c r="UL17" s="47"/>
-      <c r="UM17" s="47"/>
-      <c r="UN17" s="47"/>
-      <c r="UO17" s="47"/>
-      <c r="UP17" s="47"/>
-      <c r="UQ17" s="47"/>
-      <c r="UR17" s="47"/>
-      <c r="US17" s="47"/>
-      <c r="UT17" s="47"/>
-      <c r="UU17" s="47"/>
-      <c r="UV17" s="47"/>
-      <c r="UW17" s="47"/>
-      <c r="UX17" s="47"/>
-      <c r="UY17" s="47"/>
-      <c r="UZ17" s="47"/>
-      <c r="VA17" s="47"/>
-      <c r="VB17" s="47"/>
-      <c r="VC17" s="47"/>
-      <c r="VD17" s="47"/>
-      <c r="VE17" s="47"/>
-      <c r="VF17" s="47"/>
-      <c r="VG17" s="47"/>
-      <c r="VH17" s="47"/>
-      <c r="VI17" s="47"/>
-      <c r="VJ17" s="47"/>
-      <c r="VK17" s="47"/>
-      <c r="VL17" s="47"/>
-      <c r="VM17" s="47"/>
-      <c r="VN17" s="47"/>
-      <c r="VO17" s="47"/>
-      <c r="VP17" s="47"/>
-      <c r="VQ17" s="47"/>
-      <c r="VR17" s="47"/>
-      <c r="VS17" s="47"/>
-      <c r="VT17" s="47"/>
-      <c r="VU17" s="47"/>
-      <c r="VV17" s="47"/>
-      <c r="VW17" s="47"/>
-      <c r="VX17" s="47"/>
-      <c r="VY17" s="47"/>
-      <c r="VZ17" s="47"/>
-      <c r="WA17" s="47"/>
-      <c r="WB17" s="47"/>
-      <c r="WC17" s="47"/>
-      <c r="WD17" s="47"/>
-      <c r="WE17" s="47"/>
-      <c r="WF17" s="47"/>
-      <c r="WG17" s="47"/>
-      <c r="WH17" s="47"/>
-      <c r="WI17" s="47"/>
-      <c r="WJ17" s="47"/>
-      <c r="WK17" s="47"/>
-      <c r="WL17" s="47"/>
-      <c r="WM17" s="47"/>
-      <c r="WN17" s="47"/>
-      <c r="WO17" s="47"/>
-      <c r="WP17" s="47"/>
-      <c r="WQ17" s="47"/>
-      <c r="WR17" s="47"/>
-      <c r="WS17" s="47"/>
-      <c r="WT17" s="47"/>
-      <c r="WU17" s="47"/>
-      <c r="WV17" s="47"/>
-      <c r="WW17" s="47"/>
-      <c r="WX17" s="47"/>
-      <c r="WY17" s="47"/>
-      <c r="WZ17" s="47"/>
-      <c r="XA17" s="47"/>
-      <c r="XB17" s="47"/>
-      <c r="XC17" s="47"/>
-      <c r="XD17" s="47"/>
-      <c r="XE17" s="47"/>
-      <c r="XF17" s="47"/>
-      <c r="XG17" s="47"/>
-      <c r="XH17" s="47"/>
-      <c r="XI17" s="47"/>
-      <c r="XJ17" s="47"/>
-      <c r="XK17" s="47"/>
-      <c r="XL17" s="47"/>
-      <c r="XM17" s="47"/>
-      <c r="XN17" s="47"/>
-      <c r="XO17" s="47"/>
-      <c r="XP17" s="47"/>
-      <c r="XQ17" s="47"/>
-      <c r="XR17" s="47"/>
-      <c r="XS17" s="47"/>
-      <c r="XT17" s="47"/>
-      <c r="XU17" s="47"/>
-      <c r="XV17" s="47"/>
-      <c r="XW17" s="47"/>
-      <c r="XX17" s="47"/>
-      <c r="XY17" s="47"/>
-      <c r="XZ17" s="47"/>
-      <c r="YA17" s="47"/>
-      <c r="YB17" s="47"/>
-      <c r="YC17" s="47"/>
-      <c r="YD17" s="47"/>
-      <c r="YE17" s="47"/>
-      <c r="YF17" s="47"/>
-      <c r="YG17" s="47"/>
-      <c r="YH17" s="47"/>
-      <c r="YI17" s="47"/>
-      <c r="YJ17" s="47"/>
-      <c r="YK17" s="47"/>
-      <c r="YL17" s="47"/>
-      <c r="YM17" s="47"/>
-      <c r="YN17" s="47"/>
-      <c r="YO17" s="47"/>
-      <c r="YP17" s="47"/>
-      <c r="YQ17" s="47"/>
-      <c r="YR17" s="47"/>
-      <c r="YS17" s="47"/>
-      <c r="YT17" s="47"/>
-      <c r="YU17" s="47"/>
-      <c r="YV17" s="47"/>
-      <c r="YW17" s="47"/>
-      <c r="YX17" s="47"/>
-      <c r="YY17" s="47"/>
-      <c r="YZ17" s="47"/>
-      <c r="ZA17" s="47"/>
-      <c r="ZB17" s="47"/>
-      <c r="ZC17" s="47"/>
-      <c r="ZD17" s="47"/>
-      <c r="ZE17" s="47"/>
-      <c r="ZF17" s="47"/>
-      <c r="ZG17" s="47"/>
-      <c r="ZH17" s="47"/>
-      <c r="ZI17" s="47"/>
-      <c r="ZJ17" s="47"/>
-      <c r="ZK17" s="47"/>
-      <c r="ZL17" s="47"/>
-      <c r="ZM17" s="47"/>
-      <c r="ZN17" s="47"/>
-      <c r="ZO17" s="47"/>
-      <c r="ZP17" s="47"/>
-      <c r="ZQ17" s="47"/>
-      <c r="ZR17" s="47"/>
-      <c r="ZS17" s="47"/>
-      <c r="ZT17" s="47"/>
-      <c r="ZU17" s="47"/>
-      <c r="ZV17" s="47"/>
-      <c r="ZW17" s="47"/>
-      <c r="ZX17" s="47"/>
-      <c r="ZY17" s="47"/>
-      <c r="ZZ17" s="47"/>
-      <c r="AAA17" s="47"/>
-      <c r="AAB17" s="47"/>
-      <c r="AAC17" s="47"/>
-      <c r="AAD17" s="47"/>
-      <c r="AAE17" s="47"/>
-      <c r="AAF17" s="47"/>
-      <c r="AAG17" s="47"/>
-      <c r="AAH17" s="47"/>
-      <c r="AAI17" s="47"/>
-      <c r="AAJ17" s="47"/>
-      <c r="AAK17" s="47"/>
-      <c r="AAL17" s="47"/>
-      <c r="AAM17" s="47"/>
-      <c r="AAN17" s="47"/>
-      <c r="AAO17" s="47"/>
-      <c r="AAP17" s="47"/>
-      <c r="AAQ17" s="47"/>
-      <c r="AAR17" s="47"/>
-      <c r="AAS17" s="47"/>
-      <c r="AAT17" s="47"/>
-      <c r="AAU17" s="47"/>
-      <c r="AAV17" s="47"/>
-      <c r="AAW17" s="47"/>
-      <c r="AAX17" s="47"/>
-      <c r="AAY17" s="47"/>
-      <c r="AAZ17" s="47"/>
-      <c r="ABA17" s="47"/>
-      <c r="ABB17" s="47"/>
-      <c r="ABC17" s="47"/>
-      <c r="ABD17" s="47"/>
-      <c r="ABE17" s="47"/>
-      <c r="ABF17" s="47"/>
-      <c r="ABG17" s="47"/>
-      <c r="ABH17" s="47"/>
-      <c r="ABI17" s="47"/>
-      <c r="ABJ17" s="47"/>
-      <c r="ABK17" s="47"/>
-      <c r="ABL17" s="47"/>
-      <c r="ABM17" s="47"/>
-      <c r="ABN17" s="47"/>
-      <c r="ABO17" s="47"/>
-      <c r="ABP17" s="47"/>
-      <c r="ABQ17" s="47"/>
-      <c r="ABR17" s="47"/>
-      <c r="ABS17" s="47"/>
-      <c r="ABT17" s="47"/>
-      <c r="ABU17" s="47"/>
-      <c r="ABV17" s="47"/>
-      <c r="ABW17" s="47"/>
-      <c r="ABX17" s="47"/>
-      <c r="ABY17" s="47"/>
-      <c r="ABZ17" s="47"/>
-      <c r="ACA17" s="47"/>
-      <c r="ACB17" s="47"/>
-      <c r="ACC17" s="47"/>
-      <c r="ACD17" s="47"/>
-      <c r="ACE17" s="47"/>
-      <c r="ACF17" s="47"/>
-      <c r="ACG17" s="47"/>
-      <c r="ACH17" s="47"/>
-      <c r="ACI17" s="47"/>
-      <c r="ACJ17" s="47"/>
-      <c r="ACK17" s="47"/>
-      <c r="ACL17" s="47"/>
-      <c r="ACM17" s="47"/>
-      <c r="ACN17" s="47"/>
-      <c r="ACO17" s="47"/>
-      <c r="ACP17" s="47"/>
-      <c r="ACQ17" s="47"/>
-      <c r="ACR17" s="47"/>
-      <c r="ACS17" s="47"/>
-      <c r="ACT17" s="47"/>
-      <c r="ACU17" s="47"/>
-      <c r="ACV17" s="47"/>
-      <c r="ACW17" s="47"/>
-      <c r="ACX17" s="47"/>
-      <c r="ACY17" s="47"/>
-      <c r="ACZ17" s="47"/>
-      <c r="ADA17" s="47"/>
-      <c r="ADB17" s="47"/>
-      <c r="ADC17" s="47"/>
-      <c r="ADD17" s="47"/>
-      <c r="ADE17" s="47"/>
-      <c r="ADF17" s="47"/>
-      <c r="ADG17" s="47"/>
-      <c r="ADH17" s="47"/>
-      <c r="ADI17" s="47"/>
-      <c r="ADJ17" s="47"/>
-      <c r="ADK17" s="47"/>
-      <c r="ADL17" s="47"/>
-      <c r="ADM17" s="47"/>
-      <c r="ADN17" s="47"/>
-      <c r="ADO17" s="47"/>
-      <c r="ADP17" s="47"/>
-      <c r="ADQ17" s="47"/>
-      <c r="ADR17" s="47"/>
-      <c r="ADS17" s="47"/>
-      <c r="ADT17" s="47"/>
-      <c r="ADU17" s="47"/>
-      <c r="ADV17" s="47"/>
-      <c r="ADW17" s="47"/>
-      <c r="ADX17" s="47"/>
-      <c r="ADY17" s="47"/>
-      <c r="ADZ17" s="47"/>
-      <c r="AEA17" s="47"/>
-      <c r="AEB17" s="47"/>
-      <c r="AEC17" s="47"/>
-      <c r="AED17" s="47"/>
-      <c r="AEE17" s="47"/>
-      <c r="AEF17" s="47"/>
-      <c r="AEG17" s="47"/>
-      <c r="AEH17" s="47"/>
-      <c r="AEI17" s="47"/>
-      <c r="AEJ17" s="47"/>
-      <c r="AEK17" s="47"/>
-      <c r="AEL17" s="47"/>
-      <c r="AEM17" s="47"/>
-      <c r="AEN17" s="47"/>
-      <c r="AEO17" s="47"/>
-      <c r="AEP17" s="47"/>
-      <c r="AEQ17" s="47"/>
-      <c r="AER17" s="47"/>
-      <c r="AES17" s="47"/>
-      <c r="AET17" s="47"/>
-      <c r="AEU17" s="47"/>
-      <c r="AEV17" s="47"/>
-      <c r="AEW17" s="47"/>
-      <c r="AEX17" s="47"/>
-      <c r="AEY17" s="47"/>
-      <c r="AEZ17" s="47"/>
-      <c r="AFA17" s="47"/>
-      <c r="AFB17" s="47"/>
-      <c r="AFC17" s="47"/>
-      <c r="AFD17" s="47"/>
-      <c r="AFE17" s="47"/>
-      <c r="AFF17" s="47"/>
-      <c r="AFG17" s="47"/>
-      <c r="AFH17" s="47"/>
-      <c r="AFI17" s="47"/>
-      <c r="AFJ17" s="47"/>
-      <c r="AFK17" s="47"/>
-      <c r="AFL17" s="47"/>
-      <c r="AFM17" s="47"/>
-      <c r="AFN17" s="47"/>
-      <c r="AFO17" s="47"/>
-      <c r="AFP17" s="47"/>
-      <c r="AFQ17" s="47"/>
-      <c r="AFR17" s="47"/>
-      <c r="AFS17" s="47"/>
-      <c r="AFT17" s="47"/>
-      <c r="AFU17" s="47"/>
-      <c r="AFV17" s="47"/>
-      <c r="AFW17" s="47"/>
-      <c r="AFX17" s="47"/>
-      <c r="AFY17" s="47"/>
-      <c r="AFZ17" s="47"/>
-      <c r="AGA17" s="47"/>
-      <c r="AGB17" s="47"/>
-      <c r="AGC17" s="47"/>
-      <c r="AGD17" s="47"/>
-      <c r="AGE17" s="47"/>
-      <c r="AGF17" s="47"/>
-      <c r="AGG17" s="47"/>
-      <c r="AGH17" s="47"/>
-      <c r="AGI17" s="47"/>
-      <c r="AGJ17" s="47"/>
-      <c r="AGK17" s="47"/>
-      <c r="AGL17" s="47"/>
-      <c r="AGM17" s="47"/>
-      <c r="AGN17" s="47"/>
-      <c r="AGO17" s="47"/>
-      <c r="AGP17" s="47"/>
-      <c r="AGQ17" s="47"/>
-      <c r="AGR17" s="47"/>
-      <c r="AGS17" s="47"/>
-      <c r="AGT17" s="47"/>
-      <c r="AGU17" s="47"/>
-      <c r="AGV17" s="47"/>
-      <c r="AGW17" s="47"/>
-      <c r="AGX17" s="47"/>
-      <c r="AGY17" s="47"/>
-      <c r="AGZ17" s="47"/>
-      <c r="AHA17" s="47"/>
-      <c r="AHB17" s="47"/>
-      <c r="AHC17" s="47"/>
-      <c r="AHD17" s="47"/>
-      <c r="AHE17" s="47"/>
-      <c r="AHF17" s="47"/>
-      <c r="AHG17" s="47"/>
-      <c r="AHH17" s="47"/>
-      <c r="AHI17" s="47"/>
-      <c r="AHJ17" s="47"/>
-      <c r="AHK17" s="47"/>
-      <c r="AHL17" s="47"/>
-      <c r="AHM17" s="47"/>
-      <c r="AHN17" s="47"/>
-      <c r="AHO17" s="47"/>
-      <c r="AHP17" s="47"/>
-      <c r="AHQ17" s="47"/>
-      <c r="AHR17" s="47"/>
-      <c r="AHS17" s="47"/>
-      <c r="AHT17" s="47"/>
-      <c r="AHU17" s="47"/>
-      <c r="AHV17" s="47"/>
-      <c r="AHW17" s="47"/>
-      <c r="AHX17" s="47"/>
-      <c r="AHY17" s="47"/>
-      <c r="AHZ17" s="47"/>
-      <c r="AIA17" s="47"/>
-      <c r="AIB17" s="47"/>
-      <c r="AIC17" s="47"/>
-      <c r="AID17" s="47"/>
-      <c r="AIE17" s="47"/>
-      <c r="AIF17" s="47"/>
-      <c r="AIG17" s="47"/>
-      <c r="AIH17" s="47"/>
-      <c r="AII17" s="47"/>
-      <c r="AIJ17" s="47"/>
-      <c r="AIK17" s="47"/>
-      <c r="AIL17" s="47"/>
-      <c r="AIM17" s="47"/>
-      <c r="AIN17" s="47"/>
-      <c r="AIO17" s="47"/>
-      <c r="AIP17" s="47"/>
-      <c r="AIQ17" s="47"/>
-      <c r="AIR17" s="47"/>
-      <c r="AIS17" s="47"/>
-      <c r="AIT17" s="47"/>
-      <c r="AIU17" s="47"/>
-      <c r="AIV17" s="47"/>
-      <c r="AIW17" s="47"/>
-      <c r="AIX17" s="47"/>
-      <c r="AIY17" s="47"/>
-      <c r="AIZ17" s="47"/>
-      <c r="AJA17" s="47"/>
-      <c r="AJB17" s="47"/>
-      <c r="AJC17" s="47"/>
-      <c r="AJD17" s="47"/>
-      <c r="AJE17" s="47"/>
-      <c r="AJF17" s="47"/>
-      <c r="AJG17" s="47"/>
-      <c r="AJH17" s="47"/>
-      <c r="AJI17" s="47"/>
-      <c r="AJJ17" s="47"/>
-      <c r="AJK17" s="47"/>
-      <c r="AJL17" s="47"/>
-      <c r="AJM17" s="47"/>
-      <c r="AJN17" s="47"/>
-      <c r="AJO17" s="47"/>
-      <c r="AJP17" s="47"/>
-      <c r="AJQ17" s="47"/>
-      <c r="AJR17" s="47"/>
-      <c r="AJS17" s="47"/>
-      <c r="AJT17" s="47"/>
-      <c r="AJU17" s="47"/>
-      <c r="AJV17" s="47"/>
-      <c r="AJW17" s="47"/>
-      <c r="AJX17" s="47"/>
-      <c r="AJY17" s="47"/>
-      <c r="AJZ17" s="47"/>
-      <c r="AKA17" s="47"/>
-      <c r="AKB17" s="47"/>
-      <c r="AKC17" s="47"/>
-      <c r="AKD17" s="47"/>
-      <c r="AKE17" s="47"/>
-      <c r="AKF17" s="47"/>
-      <c r="AKG17" s="47"/>
-      <c r="AKH17" s="47"/>
-      <c r="AKI17" s="47"/>
-      <c r="AKJ17" s="47"/>
-      <c r="AKK17" s="47"/>
-      <c r="AKL17" s="47"/>
-      <c r="AKM17" s="47"/>
-      <c r="AKN17" s="47"/>
-      <c r="AKO17" s="47"/>
-      <c r="AKP17" s="47"/>
-      <c r="AKQ17" s="47"/>
-      <c r="AKR17" s="47"/>
-      <c r="AKS17" s="47"/>
-      <c r="AKT17" s="47"/>
-      <c r="AKU17" s="47"/>
-      <c r="AKV17" s="47"/>
-      <c r="AKW17" s="47"/>
-      <c r="AKX17" s="47"/>
-      <c r="AKY17" s="47"/>
-      <c r="AKZ17" s="47"/>
-      <c r="ALA17" s="47"/>
-      <c r="ALB17" s="47"/>
-      <c r="ALC17" s="47"/>
-      <c r="ALD17" s="47"/>
-      <c r="ALE17" s="47"/>
-      <c r="ALF17" s="47"/>
-      <c r="ALG17" s="47"/>
-      <c r="ALH17" s="47"/>
-      <c r="ALI17" s="47"/>
-      <c r="ALJ17" s="47"/>
-      <c r="ALK17" s="47"/>
-      <c r="ALL17" s="47"/>
-      <c r="ALM17" s="47"/>
-      <c r="ALN17" s="47"/>
-      <c r="ALO17" s="47"/>
-      <c r="ALP17" s="47"/>
-      <c r="ALQ17" s="47"/>
-      <c r="ALR17" s="47"/>
-      <c r="ALS17" s="47"/>
-      <c r="ALT17" s="47"/>
-      <c r="ALU17" s="47"/>
-      <c r="ALV17" s="47"/>
-      <c r="ALW17" s="47"/>
-      <c r="ALX17" s="47"/>
-      <c r="ALY17" s="47"/>
-      <c r="ALZ17" s="47"/>
-      <c r="AMA17" s="47"/>
-      <c r="AMB17" s="47"/>
-      <c r="AMC17" s="47"/>
-      <c r="AMD17" s="47"/>
-      <c r="AME17" s="47"/>
-      <c r="AMF17" s="47"/>
-      <c r="AMG17" s="47"/>
-      <c r="AMH17" s="47"/>
-      <c r="AMI17" s="47"/>
-      <c r="AMJ17" s="47"/>
-      <c r="AMK17" s="47"/>
-      <c r="AML17" s="47"/>
-      <c r="AMM17" s="47"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="53"/>
+      <c r="Z17" s="53"/>
+      <c r="AA17" s="53"/>
+      <c r="AB17" s="53"/>
+      <c r="AC17" s="53"/>
+      <c r="AD17" s="53"/>
+      <c r="AE17" s="53"/>
+      <c r="AF17" s="53"/>
+      <c r="AG17" s="53"/>
+      <c r="AH17" s="53"/>
+      <c r="AI17" s="53"/>
+      <c r="AJ17" s="53"/>
+      <c r="AK17" s="53"/>
+      <c r="AL17" s="53"/>
+      <c r="AM17" s="53"/>
+      <c r="AN17" s="53"/>
+      <c r="AO17" s="53"/>
+      <c r="AP17" s="53"/>
+      <c r="AQ17" s="53"/>
+      <c r="AR17" s="53"/>
+      <c r="AS17" s="53"/>
+      <c r="AT17" s="53"/>
+      <c r="AU17" s="53"/>
+      <c r="AV17" s="53"/>
+      <c r="AW17" s="53"/>
+      <c r="AX17" s="53"/>
+      <c r="AY17" s="53"/>
+      <c r="AZ17" s="53"/>
+      <c r="BA17" s="53"/>
+      <c r="BB17" s="53"/>
+      <c r="BC17" s="53"/>
+      <c r="BD17" s="53"/>
+      <c r="BE17" s="53"/>
+      <c r="BF17" s="53"/>
+      <c r="BG17" s="53"/>
+      <c r="BH17" s="53"/>
+      <c r="BI17" s="53"/>
+      <c r="BJ17" s="53"/>
+      <c r="BK17" s="53"/>
+      <c r="BL17" s="53"/>
+      <c r="BM17" s="53"/>
+      <c r="BN17" s="53"/>
+      <c r="BO17" s="53"/>
+      <c r="BP17" s="53"/>
+      <c r="BQ17" s="53"/>
+      <c r="BR17" s="53"/>
+      <c r="BS17" s="53"/>
+      <c r="BT17" s="53"/>
+      <c r="BU17" s="53"/>
+      <c r="BV17" s="53"/>
+      <c r="BW17" s="53"/>
+      <c r="BX17" s="53"/>
+      <c r="BY17" s="53"/>
+      <c r="BZ17" s="53"/>
+      <c r="CA17" s="53"/>
+      <c r="CB17" s="53"/>
+      <c r="CC17" s="53"/>
+      <c r="CD17" s="53"/>
+      <c r="CE17" s="53"/>
+      <c r="CF17" s="53"/>
+      <c r="CG17" s="53"/>
+      <c r="CH17" s="53"/>
+      <c r="CI17" s="53"/>
+      <c r="CJ17" s="53"/>
+      <c r="CK17" s="53"/>
+      <c r="CL17" s="53"/>
+      <c r="CM17" s="53"/>
+      <c r="CN17" s="53"/>
+      <c r="CO17" s="53"/>
+      <c r="CP17" s="53"/>
+      <c r="CQ17" s="53"/>
+      <c r="CR17" s="53"/>
+      <c r="CS17" s="53"/>
+      <c r="CT17" s="53"/>
+      <c r="CU17" s="53"/>
+      <c r="CV17" s="53"/>
+      <c r="CW17" s="53"/>
+      <c r="CX17" s="53"/>
+      <c r="CY17" s="53"/>
+      <c r="CZ17" s="53"/>
+      <c r="DA17" s="53"/>
+      <c r="DB17" s="53"/>
+      <c r="DC17" s="53"/>
+      <c r="DD17" s="53"/>
+      <c r="DE17" s="53"/>
+      <c r="DF17" s="53"/>
+      <c r="DG17" s="53"/>
+      <c r="DH17" s="53"/>
+      <c r="DI17" s="53"/>
+      <c r="DJ17" s="53"/>
+      <c r="DK17" s="53"/>
+      <c r="DL17" s="53"/>
+      <c r="DM17" s="53"/>
+      <c r="DN17" s="53"/>
+      <c r="DO17" s="53"/>
+      <c r="DP17" s="53"/>
+      <c r="DQ17" s="53"/>
+      <c r="DR17" s="53"/>
+      <c r="DS17" s="53"/>
+      <c r="DT17" s="53"/>
+      <c r="DU17" s="53"/>
+      <c r="DV17" s="53"/>
+      <c r="DW17" s="53"/>
+      <c r="DX17" s="53"/>
+      <c r="DY17" s="53"/>
+      <c r="DZ17" s="53"/>
+      <c r="EA17" s="53"/>
+      <c r="EB17" s="53"/>
+      <c r="EC17" s="53"/>
+      <c r="ED17" s="53"/>
+      <c r="EE17" s="53"/>
+      <c r="EF17" s="53"/>
+      <c r="EG17" s="53"/>
+      <c r="EH17" s="53"/>
+      <c r="EI17" s="53"/>
+      <c r="EJ17" s="53"/>
+      <c r="EK17" s="53"/>
+      <c r="EL17" s="53"/>
+      <c r="EM17" s="53"/>
+      <c r="EN17" s="53"/>
+      <c r="EO17" s="53"/>
+      <c r="EP17" s="53"/>
+      <c r="EQ17" s="53"/>
+      <c r="ER17" s="53"/>
+      <c r="ES17" s="53"/>
+      <c r="ET17" s="53"/>
+      <c r="EU17" s="53"/>
+      <c r="EV17" s="53"/>
+      <c r="EW17" s="53"/>
+      <c r="EX17" s="53"/>
+      <c r="EY17" s="53"/>
+      <c r="EZ17" s="53"/>
+      <c r="FA17" s="53"/>
+      <c r="FB17" s="53"/>
+      <c r="FC17" s="53"/>
+      <c r="FD17" s="53"/>
+      <c r="FE17" s="53"/>
+      <c r="FF17" s="53"/>
+      <c r="FG17" s="53"/>
+      <c r="FH17" s="53"/>
+      <c r="FI17" s="53"/>
+      <c r="FJ17" s="53"/>
+      <c r="FK17" s="53"/>
+      <c r="FL17" s="53"/>
+      <c r="FM17" s="53"/>
+      <c r="FN17" s="53"/>
+      <c r="FO17" s="53"/>
+      <c r="FP17" s="53"/>
+      <c r="FQ17" s="53"/>
+      <c r="FR17" s="53"/>
+      <c r="FS17" s="53"/>
+      <c r="FT17" s="53"/>
+      <c r="FU17" s="53"/>
+      <c r="FV17" s="53"/>
+      <c r="FW17" s="53"/>
+      <c r="FX17" s="53"/>
+      <c r="FY17" s="53"/>
+      <c r="FZ17" s="53"/>
+      <c r="GA17" s="53"/>
+      <c r="GB17" s="53"/>
+      <c r="GC17" s="53"/>
+      <c r="GD17" s="53"/>
+      <c r="GE17" s="53"/>
+      <c r="GF17" s="53"/>
+      <c r="GG17" s="53"/>
+      <c r="GH17" s="53"/>
+      <c r="GI17" s="53"/>
+      <c r="GJ17" s="53"/>
+      <c r="GK17" s="53"/>
+      <c r="GL17" s="53"/>
+      <c r="GM17" s="53"/>
+      <c r="GN17" s="53"/>
+      <c r="GO17" s="53"/>
+      <c r="GP17" s="53"/>
+      <c r="GQ17" s="53"/>
+      <c r="GR17" s="53"/>
+      <c r="GS17" s="53"/>
+      <c r="GT17" s="53"/>
+      <c r="GU17" s="53"/>
+      <c r="GV17" s="53"/>
+      <c r="GW17" s="53"/>
+      <c r="GX17" s="53"/>
+      <c r="GY17" s="53"/>
+      <c r="GZ17" s="53"/>
+      <c r="HA17" s="53"/>
+      <c r="HB17" s="53"/>
+      <c r="HC17" s="53"/>
+      <c r="HD17" s="53"/>
+      <c r="HE17" s="53"/>
+      <c r="HF17" s="53"/>
+      <c r="HG17" s="53"/>
+      <c r="HH17" s="53"/>
+      <c r="HI17" s="53"/>
+      <c r="HJ17" s="53"/>
+      <c r="HK17" s="53"/>
+      <c r="HL17" s="53"/>
+      <c r="HM17" s="53"/>
+      <c r="HN17" s="53"/>
+      <c r="HO17" s="53"/>
+      <c r="HP17" s="53"/>
+      <c r="HQ17" s="53"/>
+      <c r="HR17" s="53"/>
+      <c r="HS17" s="53"/>
+      <c r="HT17" s="53"/>
+      <c r="HU17" s="53"/>
+      <c r="HV17" s="53"/>
+      <c r="HW17" s="53"/>
+      <c r="HX17" s="53"/>
+      <c r="HY17" s="53"/>
+      <c r="HZ17" s="53"/>
+      <c r="IA17" s="53"/>
+      <c r="IB17" s="53"/>
+      <c r="IC17" s="53"/>
+      <c r="ID17" s="53"/>
+      <c r="IE17" s="53"/>
+      <c r="IF17" s="53"/>
+      <c r="IG17" s="53"/>
+      <c r="IH17" s="53"/>
+      <c r="II17" s="53"/>
+      <c r="IJ17" s="53"/>
+      <c r="IK17" s="53"/>
+      <c r="IL17" s="53"/>
+      <c r="IM17" s="53"/>
+      <c r="IN17" s="53"/>
+      <c r="IO17" s="53"/>
+      <c r="IP17" s="53"/>
+      <c r="IQ17" s="53"/>
+      <c r="IR17" s="53"/>
+      <c r="IS17" s="53"/>
+      <c r="IT17" s="53"/>
+      <c r="IU17" s="53"/>
+      <c r="IV17" s="53"/>
+      <c r="IW17" s="53"/>
+      <c r="IX17" s="53"/>
+      <c r="IY17" s="53"/>
+      <c r="IZ17" s="53"/>
+      <c r="JA17" s="53"/>
+      <c r="JB17" s="53"/>
+      <c r="JC17" s="53"/>
+      <c r="JD17" s="53"/>
+      <c r="JE17" s="53"/>
+      <c r="JF17" s="53"/>
+      <c r="JG17" s="53"/>
+      <c r="JH17" s="53"/>
+      <c r="JI17" s="53"/>
+      <c r="JJ17" s="53"/>
+      <c r="JK17" s="53"/>
+      <c r="JL17" s="53"/>
+      <c r="JM17" s="53"/>
+      <c r="JN17" s="53"/>
+      <c r="JO17" s="53"/>
+      <c r="JP17" s="53"/>
+      <c r="JQ17" s="53"/>
+      <c r="JR17" s="53"/>
+      <c r="JS17" s="53"/>
+      <c r="JT17" s="53"/>
+      <c r="JU17" s="53"/>
+      <c r="JV17" s="53"/>
+      <c r="JW17" s="53"/>
+      <c r="JX17" s="53"/>
+      <c r="JY17" s="53"/>
+      <c r="JZ17" s="53"/>
+      <c r="KA17" s="53"/>
+      <c r="KB17" s="53"/>
+      <c r="KC17" s="53"/>
+      <c r="KD17" s="53"/>
+      <c r="KE17" s="53"/>
+      <c r="KF17" s="53"/>
+      <c r="KG17" s="53"/>
+      <c r="KH17" s="53"/>
+      <c r="KI17" s="53"/>
+      <c r="KJ17" s="53"/>
+      <c r="KK17" s="53"/>
+      <c r="KL17" s="53"/>
+      <c r="KM17" s="53"/>
+      <c r="KN17" s="53"/>
+      <c r="KO17" s="53"/>
+      <c r="KP17" s="53"/>
+      <c r="KQ17" s="53"/>
+      <c r="KR17" s="53"/>
+      <c r="KS17" s="53"/>
+      <c r="KT17" s="53"/>
+      <c r="KU17" s="53"/>
+      <c r="KV17" s="53"/>
+      <c r="KW17" s="53"/>
+      <c r="KX17" s="53"/>
+      <c r="KY17" s="53"/>
+      <c r="KZ17" s="53"/>
+      <c r="LA17" s="53"/>
+      <c r="LB17" s="53"/>
+      <c r="LC17" s="53"/>
+      <c r="LD17" s="53"/>
+      <c r="LE17" s="53"/>
+      <c r="LF17" s="53"/>
+      <c r="LG17" s="53"/>
+      <c r="LH17" s="53"/>
+      <c r="LI17" s="53"/>
+      <c r="LJ17" s="53"/>
+      <c r="LK17" s="53"/>
+      <c r="LL17" s="53"/>
+      <c r="LM17" s="53"/>
+      <c r="LN17" s="53"/>
+      <c r="LO17" s="53"/>
+      <c r="LP17" s="53"/>
+      <c r="LQ17" s="53"/>
+      <c r="LR17" s="53"/>
+      <c r="LS17" s="53"/>
+      <c r="LT17" s="53"/>
+      <c r="LU17" s="53"/>
+      <c r="LV17" s="53"/>
+      <c r="LW17" s="53"/>
+      <c r="LX17" s="53"/>
+      <c r="LY17" s="53"/>
+      <c r="LZ17" s="53"/>
+      <c r="MA17" s="53"/>
+      <c r="MB17" s="53"/>
+      <c r="MC17" s="53"/>
+      <c r="MD17" s="53"/>
+      <c r="ME17" s="53"/>
+      <c r="MF17" s="53"/>
+      <c r="MG17" s="53"/>
+      <c r="MH17" s="53"/>
+      <c r="MI17" s="53"/>
+      <c r="MJ17" s="53"/>
+      <c r="MK17" s="53"/>
+      <c r="ML17" s="53"/>
+      <c r="MM17" s="53"/>
+      <c r="MN17" s="53"/>
+      <c r="MO17" s="53"/>
+      <c r="MP17" s="53"/>
+      <c r="MQ17" s="53"/>
+      <c r="MR17" s="53"/>
+      <c r="MS17" s="53"/>
+      <c r="MT17" s="53"/>
+      <c r="MU17" s="53"/>
+      <c r="MV17" s="53"/>
+      <c r="MW17" s="53"/>
+      <c r="MX17" s="53"/>
+      <c r="MY17" s="53"/>
+      <c r="MZ17" s="53"/>
+      <c r="NA17" s="53"/>
+      <c r="NB17" s="53"/>
+      <c r="NC17" s="53"/>
+      <c r="ND17" s="53"/>
+      <c r="NE17" s="53"/>
+      <c r="NF17" s="53"/>
+      <c r="NG17" s="53"/>
+      <c r="NH17" s="53"/>
+      <c r="NI17" s="53"/>
+      <c r="NJ17" s="53"/>
+      <c r="NK17" s="53"/>
+      <c r="NL17" s="53"/>
+      <c r="NM17" s="53"/>
+      <c r="NN17" s="53"/>
+      <c r="NO17" s="53"/>
+      <c r="NP17" s="53"/>
+      <c r="NQ17" s="53"/>
+      <c r="NR17" s="53"/>
+      <c r="NS17" s="53"/>
+      <c r="NT17" s="53"/>
+      <c r="NU17" s="53"/>
+      <c r="NV17" s="53"/>
+      <c r="NW17" s="53"/>
+      <c r="NX17" s="53"/>
+      <c r="NY17" s="53"/>
+      <c r="NZ17" s="53"/>
+      <c r="OA17" s="53"/>
+      <c r="OB17" s="53"/>
+      <c r="OC17" s="53"/>
+      <c r="OD17" s="53"/>
+      <c r="OE17" s="53"/>
+      <c r="OF17" s="53"/>
+      <c r="OG17" s="53"/>
+      <c r="OH17" s="53"/>
+      <c r="OI17" s="53"/>
+      <c r="OJ17" s="53"/>
+      <c r="OK17" s="53"/>
+      <c r="OL17" s="53"/>
+      <c r="OM17" s="53"/>
+      <c r="ON17" s="53"/>
+      <c r="OO17" s="53"/>
+      <c r="OP17" s="53"/>
+      <c r="OQ17" s="53"/>
+      <c r="OR17" s="53"/>
+      <c r="OS17" s="53"/>
+      <c r="OT17" s="53"/>
+      <c r="OU17" s="53"/>
+      <c r="OV17" s="53"/>
+      <c r="OW17" s="53"/>
+      <c r="OX17" s="53"/>
+      <c r="OY17" s="53"/>
+      <c r="OZ17" s="53"/>
+      <c r="PA17" s="53"/>
+      <c r="PB17" s="53"/>
+      <c r="PC17" s="53"/>
+      <c r="PD17" s="53"/>
+      <c r="PE17" s="53"/>
+      <c r="PF17" s="53"/>
+      <c r="PG17" s="53"/>
+      <c r="PH17" s="53"/>
+      <c r="PI17" s="53"/>
+      <c r="PJ17" s="53"/>
+      <c r="PK17" s="53"/>
+      <c r="PL17" s="53"/>
+      <c r="PM17" s="53"/>
+      <c r="PN17" s="53"/>
+      <c r="PO17" s="53"/>
+      <c r="PP17" s="53"/>
+      <c r="PQ17" s="53"/>
+      <c r="PR17" s="53"/>
+      <c r="PS17" s="53"/>
+      <c r="PT17" s="53"/>
+      <c r="PU17" s="53"/>
+      <c r="PV17" s="53"/>
+      <c r="PW17" s="53"/>
+      <c r="PX17" s="53"/>
+      <c r="PY17" s="53"/>
+      <c r="PZ17" s="53"/>
+      <c r="QA17" s="53"/>
+      <c r="QB17" s="53"/>
+      <c r="QC17" s="53"/>
+      <c r="QD17" s="53"/>
+      <c r="QE17" s="53"/>
+      <c r="QF17" s="53"/>
+      <c r="QG17" s="53"/>
+      <c r="QH17" s="53"/>
+      <c r="QI17" s="53"/>
+      <c r="QJ17" s="53"/>
+      <c r="QK17" s="53"/>
+      <c r="QL17" s="53"/>
+      <c r="QM17" s="53"/>
+      <c r="QN17" s="53"/>
+      <c r="QO17" s="53"/>
+      <c r="QP17" s="53"/>
+      <c r="QQ17" s="53"/>
+      <c r="QR17" s="53"/>
+      <c r="QS17" s="53"/>
+      <c r="QT17" s="53"/>
+      <c r="QU17" s="53"/>
+      <c r="QV17" s="53"/>
+      <c r="QW17" s="53"/>
+      <c r="QX17" s="53"/>
+      <c r="QY17" s="53"/>
+      <c r="QZ17" s="53"/>
+      <c r="RA17" s="53"/>
+      <c r="RB17" s="53"/>
+      <c r="RC17" s="53"/>
+      <c r="RD17" s="53"/>
+      <c r="RE17" s="53"/>
+      <c r="RF17" s="53"/>
+      <c r="RG17" s="53"/>
+      <c r="RH17" s="53"/>
+      <c r="RI17" s="53"/>
+      <c r="RJ17" s="53"/>
+      <c r="RK17" s="53"/>
+      <c r="RL17" s="53"/>
+      <c r="RM17" s="53"/>
+      <c r="RN17" s="53"/>
+      <c r="RO17" s="53"/>
+      <c r="RP17" s="53"/>
+      <c r="RQ17" s="53"/>
+      <c r="RR17" s="53"/>
+      <c r="RS17" s="53"/>
+      <c r="RT17" s="53"/>
+      <c r="RU17" s="53"/>
+      <c r="RV17" s="53"/>
+      <c r="RW17" s="53"/>
+      <c r="RX17" s="53"/>
+      <c r="RY17" s="53"/>
+      <c r="RZ17" s="53"/>
+      <c r="SA17" s="53"/>
+      <c r="SB17" s="53"/>
+      <c r="SC17" s="53"/>
+      <c r="SD17" s="53"/>
+      <c r="SE17" s="53"/>
+      <c r="SF17" s="53"/>
+      <c r="SG17" s="53"/>
+      <c r="SH17" s="53"/>
+      <c r="SI17" s="53"/>
+      <c r="SJ17" s="53"/>
+      <c r="SK17" s="53"/>
+      <c r="SL17" s="53"/>
+      <c r="SM17" s="53"/>
+      <c r="SN17" s="53"/>
+      <c r="SO17" s="53"/>
+      <c r="SP17" s="53"/>
+      <c r="SQ17" s="53"/>
+      <c r="SR17" s="53"/>
+      <c r="SS17" s="53"/>
+      <c r="ST17" s="53"/>
+      <c r="SU17" s="53"/>
+      <c r="SV17" s="53"/>
+      <c r="SW17" s="53"/>
+      <c r="SX17" s="53"/>
+      <c r="SY17" s="53"/>
+      <c r="SZ17" s="53"/>
+      <c r="TA17" s="53"/>
+      <c r="TB17" s="53"/>
+      <c r="TC17" s="53"/>
+      <c r="TD17" s="53"/>
+      <c r="TE17" s="53"/>
+      <c r="TF17" s="53"/>
+      <c r="TG17" s="53"/>
+      <c r="TH17" s="53"/>
+      <c r="TI17" s="53"/>
+      <c r="TJ17" s="53"/>
+      <c r="TK17" s="53"/>
+      <c r="TL17" s="53"/>
+      <c r="TM17" s="53"/>
+      <c r="TN17" s="53"/>
+      <c r="TO17" s="53"/>
+      <c r="TP17" s="53"/>
+      <c r="TQ17" s="53"/>
+      <c r="TR17" s="53"/>
+      <c r="TS17" s="53"/>
+      <c r="TT17" s="53"/>
+      <c r="TU17" s="53"/>
+      <c r="TV17" s="53"/>
+      <c r="TW17" s="53"/>
+      <c r="TX17" s="53"/>
+      <c r="TY17" s="53"/>
+      <c r="TZ17" s="53"/>
+      <c r="UA17" s="53"/>
+      <c r="UB17" s="53"/>
+      <c r="UC17" s="53"/>
+      <c r="UD17" s="53"/>
+      <c r="UE17" s="53"/>
+      <c r="UF17" s="53"/>
+      <c r="UG17" s="53"/>
+      <c r="UH17" s="53"/>
+      <c r="UI17" s="53"/>
+      <c r="UJ17" s="53"/>
+      <c r="UK17" s="53"/>
+      <c r="UL17" s="53"/>
+      <c r="UM17" s="53"/>
+      <c r="UN17" s="53"/>
+      <c r="UO17" s="53"/>
+      <c r="UP17" s="53"/>
+      <c r="UQ17" s="53"/>
+      <c r="UR17" s="53"/>
+      <c r="US17" s="53"/>
+      <c r="UT17" s="53"/>
+      <c r="UU17" s="53"/>
+      <c r="UV17" s="53"/>
+      <c r="UW17" s="53"/>
+      <c r="UX17" s="53"/>
+      <c r="UY17" s="53"/>
+      <c r="UZ17" s="53"/>
+      <c r="VA17" s="53"/>
+      <c r="VB17" s="53"/>
+      <c r="VC17" s="53"/>
+      <c r="VD17" s="53"/>
+      <c r="VE17" s="53"/>
+      <c r="VF17" s="53"/>
+      <c r="VG17" s="53"/>
+      <c r="VH17" s="53"/>
+      <c r="VI17" s="53"/>
+      <c r="VJ17" s="53"/>
+      <c r="VK17" s="53"/>
+      <c r="VL17" s="53"/>
+      <c r="VM17" s="53"/>
+      <c r="VN17" s="53"/>
+      <c r="VO17" s="53"/>
+      <c r="VP17" s="53"/>
+      <c r="VQ17" s="53"/>
+      <c r="VR17" s="53"/>
+      <c r="VS17" s="53"/>
+      <c r="VT17" s="53"/>
+      <c r="VU17" s="53"/>
+      <c r="VV17" s="53"/>
+      <c r="VW17" s="53"/>
+      <c r="VX17" s="53"/>
+      <c r="VY17" s="53"/>
+      <c r="VZ17" s="53"/>
+      <c r="WA17" s="53"/>
+      <c r="WB17" s="53"/>
+      <c r="WC17" s="53"/>
+      <c r="WD17" s="53"/>
+      <c r="WE17" s="53"/>
+      <c r="WF17" s="53"/>
+      <c r="WG17" s="53"/>
+      <c r="WH17" s="53"/>
+      <c r="WI17" s="53"/>
+      <c r="WJ17" s="53"/>
+      <c r="WK17" s="53"/>
+      <c r="WL17" s="53"/>
+      <c r="WM17" s="53"/>
+      <c r="WN17" s="53"/>
+      <c r="WO17" s="53"/>
+      <c r="WP17" s="53"/>
+      <c r="WQ17" s="53"/>
+      <c r="WR17" s="53"/>
+      <c r="WS17" s="53"/>
+      <c r="WT17" s="53"/>
+      <c r="WU17" s="53"/>
+      <c r="WV17" s="53"/>
+      <c r="WW17" s="53"/>
+      <c r="WX17" s="53"/>
+      <c r="WY17" s="53"/>
+      <c r="WZ17" s="53"/>
+      <c r="XA17" s="53"/>
+      <c r="XB17" s="53"/>
+      <c r="XC17" s="53"/>
+      <c r="XD17" s="53"/>
+      <c r="XE17" s="53"/>
+      <c r="XF17" s="53"/>
+      <c r="XG17" s="53"/>
+      <c r="XH17" s="53"/>
+      <c r="XI17" s="53"/>
+      <c r="XJ17" s="53"/>
+      <c r="XK17" s="53"/>
+      <c r="XL17" s="53"/>
+      <c r="XM17" s="53"/>
+      <c r="XN17" s="53"/>
+      <c r="XO17" s="53"/>
+      <c r="XP17" s="53"/>
+      <c r="XQ17" s="53"/>
+      <c r="XR17" s="53"/>
+      <c r="XS17" s="53"/>
+      <c r="XT17" s="53"/>
+      <c r="XU17" s="53"/>
+      <c r="XV17" s="53"/>
+      <c r="XW17" s="53"/>
+      <c r="XX17" s="53"/>
+      <c r="XY17" s="53"/>
+      <c r="XZ17" s="53"/>
+      <c r="YA17" s="53"/>
+      <c r="YB17" s="53"/>
+      <c r="YC17" s="53"/>
+      <c r="YD17" s="53"/>
+      <c r="YE17" s="53"/>
+      <c r="YF17" s="53"/>
+      <c r="YG17" s="53"/>
+      <c r="YH17" s="53"/>
+      <c r="YI17" s="53"/>
+      <c r="YJ17" s="53"/>
+      <c r="YK17" s="53"/>
+      <c r="YL17" s="53"/>
+      <c r="YM17" s="53"/>
+      <c r="YN17" s="53"/>
+      <c r="YO17" s="53"/>
+      <c r="YP17" s="53"/>
+      <c r="YQ17" s="53"/>
+      <c r="YR17" s="53"/>
+      <c r="YS17" s="53"/>
+      <c r="YT17" s="53"/>
+      <c r="YU17" s="53"/>
+      <c r="YV17" s="53"/>
+      <c r="YW17" s="53"/>
+      <c r="YX17" s="53"/>
+      <c r="YY17" s="53"/>
+      <c r="YZ17" s="53"/>
+      <c r="ZA17" s="53"/>
+      <c r="ZB17" s="53"/>
+      <c r="ZC17" s="53"/>
+      <c r="ZD17" s="53"/>
+      <c r="ZE17" s="53"/>
+      <c r="ZF17" s="53"/>
+      <c r="ZG17" s="53"/>
+      <c r="ZH17" s="53"/>
+      <c r="ZI17" s="53"/>
+      <c r="ZJ17" s="53"/>
+      <c r="ZK17" s="53"/>
+      <c r="ZL17" s="53"/>
+      <c r="ZM17" s="53"/>
+      <c r="ZN17" s="53"/>
+      <c r="ZO17" s="53"/>
+      <c r="ZP17" s="53"/>
+      <c r="ZQ17" s="53"/>
+      <c r="ZR17" s="53"/>
+      <c r="ZS17" s="53"/>
+      <c r="ZT17" s="53"/>
+      <c r="ZU17" s="53"/>
+      <c r="ZV17" s="53"/>
+      <c r="ZW17" s="53"/>
+      <c r="ZX17" s="53"/>
+      <c r="ZY17" s="53"/>
+      <c r="ZZ17" s="53"/>
+      <c r="AAA17" s="53"/>
+      <c r="AAB17" s="53"/>
+      <c r="AAC17" s="53"/>
+      <c r="AAD17" s="53"/>
+      <c r="AAE17" s="53"/>
+      <c r="AAF17" s="53"/>
+      <c r="AAG17" s="53"/>
+      <c r="AAH17" s="53"/>
+      <c r="AAI17" s="53"/>
+      <c r="AAJ17" s="53"/>
+      <c r="AAK17" s="53"/>
+      <c r="AAL17" s="53"/>
+      <c r="AAM17" s="53"/>
+      <c r="AAN17" s="53"/>
+      <c r="AAO17" s="53"/>
+      <c r="AAP17" s="53"/>
+      <c r="AAQ17" s="53"/>
+      <c r="AAR17" s="53"/>
+      <c r="AAS17" s="53"/>
+      <c r="AAT17" s="53"/>
+      <c r="AAU17" s="53"/>
+      <c r="AAV17" s="53"/>
+      <c r="AAW17" s="53"/>
+      <c r="AAX17" s="53"/>
+      <c r="AAY17" s="53"/>
+      <c r="AAZ17" s="53"/>
+      <c r="ABA17" s="53"/>
+      <c r="ABB17" s="53"/>
+      <c r="ABC17" s="53"/>
+      <c r="ABD17" s="53"/>
+      <c r="ABE17" s="53"/>
+      <c r="ABF17" s="53"/>
+      <c r="ABG17" s="53"/>
+      <c r="ABH17" s="53"/>
+      <c r="ABI17" s="53"/>
+      <c r="ABJ17" s="53"/>
+      <c r="ABK17" s="53"/>
+      <c r="ABL17" s="53"/>
+      <c r="ABM17" s="53"/>
+      <c r="ABN17" s="53"/>
+      <c r="ABO17" s="53"/>
+      <c r="ABP17" s="53"/>
+      <c r="ABQ17" s="53"/>
+      <c r="ABR17" s="53"/>
+      <c r="ABS17" s="53"/>
+      <c r="ABT17" s="53"/>
+      <c r="ABU17" s="53"/>
+      <c r="ABV17" s="53"/>
+      <c r="ABW17" s="53"/>
+      <c r="ABX17" s="53"/>
+      <c r="ABY17" s="53"/>
+      <c r="ABZ17" s="53"/>
+      <c r="ACA17" s="53"/>
+      <c r="ACB17" s="53"/>
+      <c r="ACC17" s="53"/>
+      <c r="ACD17" s="53"/>
+      <c r="ACE17" s="53"/>
+      <c r="ACF17" s="53"/>
+      <c r="ACG17" s="53"/>
+      <c r="ACH17" s="53"/>
+      <c r="ACI17" s="53"/>
+      <c r="ACJ17" s="53"/>
+      <c r="ACK17" s="53"/>
+      <c r="ACL17" s="53"/>
+      <c r="ACM17" s="53"/>
+      <c r="ACN17" s="53"/>
+      <c r="ACO17" s="53"/>
+      <c r="ACP17" s="53"/>
+      <c r="ACQ17" s="53"/>
+      <c r="ACR17" s="53"/>
+      <c r="ACS17" s="53"/>
+      <c r="ACT17" s="53"/>
+      <c r="ACU17" s="53"/>
+      <c r="ACV17" s="53"/>
+      <c r="ACW17" s="53"/>
+      <c r="ACX17" s="53"/>
+      <c r="ACY17" s="53"/>
+      <c r="ACZ17" s="53"/>
+      <c r="ADA17" s="53"/>
+      <c r="ADB17" s="53"/>
+      <c r="ADC17" s="53"/>
+      <c r="ADD17" s="53"/>
+      <c r="ADE17" s="53"/>
+      <c r="ADF17" s="53"/>
+      <c r="ADG17" s="53"/>
+      <c r="ADH17" s="53"/>
+      <c r="ADI17" s="53"/>
+      <c r="ADJ17" s="53"/>
+      <c r="ADK17" s="53"/>
+      <c r="ADL17" s="53"/>
+      <c r="ADM17" s="53"/>
+      <c r="ADN17" s="53"/>
+      <c r="ADO17" s="53"/>
+      <c r="ADP17" s="53"/>
+      <c r="ADQ17" s="53"/>
+      <c r="ADR17" s="53"/>
+      <c r="ADS17" s="53"/>
+      <c r="ADT17" s="53"/>
+      <c r="ADU17" s="53"/>
+      <c r="ADV17" s="53"/>
+      <c r="ADW17" s="53"/>
+      <c r="ADX17" s="53"/>
+      <c r="ADY17" s="53"/>
+      <c r="ADZ17" s="53"/>
+      <c r="AEA17" s="53"/>
+      <c r="AEB17" s="53"/>
+      <c r="AEC17" s="53"/>
+      <c r="AED17" s="53"/>
+      <c r="AEE17" s="53"/>
+      <c r="AEF17" s="53"/>
+      <c r="AEG17" s="53"/>
+      <c r="AEH17" s="53"/>
+      <c r="AEI17" s="53"/>
+      <c r="AEJ17" s="53"/>
+      <c r="AEK17" s="53"/>
+      <c r="AEL17" s="53"/>
+      <c r="AEM17" s="53"/>
+      <c r="AEN17" s="53"/>
+      <c r="AEO17" s="53"/>
+      <c r="AEP17" s="53"/>
+      <c r="AEQ17" s="53"/>
+      <c r="AER17" s="53"/>
+      <c r="AES17" s="53"/>
+      <c r="AET17" s="53"/>
+      <c r="AEU17" s="53"/>
+      <c r="AEV17" s="53"/>
+      <c r="AEW17" s="53"/>
+      <c r="AEX17" s="53"/>
+      <c r="AEY17" s="53"/>
+      <c r="AEZ17" s="53"/>
+      <c r="AFA17" s="53"/>
+      <c r="AFB17" s="53"/>
+      <c r="AFC17" s="53"/>
+      <c r="AFD17" s="53"/>
+      <c r="AFE17" s="53"/>
+      <c r="AFF17" s="53"/>
+      <c r="AFG17" s="53"/>
+      <c r="AFH17" s="53"/>
+      <c r="AFI17" s="53"/>
+      <c r="AFJ17" s="53"/>
+      <c r="AFK17" s="53"/>
+      <c r="AFL17" s="53"/>
+      <c r="AFM17" s="53"/>
+      <c r="AFN17" s="53"/>
+      <c r="AFO17" s="53"/>
+      <c r="AFP17" s="53"/>
+      <c r="AFQ17" s="53"/>
+      <c r="AFR17" s="53"/>
+      <c r="AFS17" s="53"/>
+      <c r="AFT17" s="53"/>
+      <c r="AFU17" s="53"/>
+      <c r="AFV17" s="53"/>
+      <c r="AFW17" s="53"/>
+      <c r="AFX17" s="53"/>
+      <c r="AFY17" s="53"/>
+      <c r="AFZ17" s="53"/>
+      <c r="AGA17" s="53"/>
+      <c r="AGB17" s="53"/>
+      <c r="AGC17" s="53"/>
+      <c r="AGD17" s="53"/>
+      <c r="AGE17" s="53"/>
+      <c r="AGF17" s="53"/>
+      <c r="AGG17" s="53"/>
+      <c r="AGH17" s="53"/>
+      <c r="AGI17" s="53"/>
+      <c r="AGJ17" s="53"/>
+      <c r="AGK17" s="53"/>
+      <c r="AGL17" s="53"/>
+      <c r="AGM17" s="53"/>
+      <c r="AGN17" s="53"/>
+      <c r="AGO17" s="53"/>
+      <c r="AGP17" s="53"/>
+      <c r="AGQ17" s="53"/>
+      <c r="AGR17" s="53"/>
+      <c r="AGS17" s="53"/>
+      <c r="AGT17" s="53"/>
+      <c r="AGU17" s="53"/>
+      <c r="AGV17" s="53"/>
+      <c r="AGW17" s="53"/>
+      <c r="AGX17" s="53"/>
+      <c r="AGY17" s="53"/>
+      <c r="AGZ17" s="53"/>
+      <c r="AHA17" s="53"/>
+      <c r="AHB17" s="53"/>
+      <c r="AHC17" s="53"/>
+      <c r="AHD17" s="53"/>
+      <c r="AHE17" s="53"/>
+      <c r="AHF17" s="53"/>
+      <c r="AHG17" s="53"/>
+      <c r="AHH17" s="53"/>
+      <c r="AHI17" s="53"/>
+      <c r="AHJ17" s="53"/>
+      <c r="AHK17" s="53"/>
+      <c r="AHL17" s="53"/>
+      <c r="AHM17" s="53"/>
+      <c r="AHN17" s="53"/>
+      <c r="AHO17" s="53"/>
+      <c r="AHP17" s="53"/>
+      <c r="AHQ17" s="53"/>
+      <c r="AHR17" s="53"/>
+      <c r="AHS17" s="53"/>
+      <c r="AHT17" s="53"/>
+      <c r="AHU17" s="53"/>
+      <c r="AHV17" s="53"/>
+      <c r="AHW17" s="53"/>
+      <c r="AHX17" s="53"/>
+      <c r="AHY17" s="53"/>
+      <c r="AHZ17" s="53"/>
+      <c r="AIA17" s="53"/>
+      <c r="AIB17" s="53"/>
+      <c r="AIC17" s="53"/>
+      <c r="AID17" s="53"/>
+      <c r="AIE17" s="53"/>
+      <c r="AIF17" s="53"/>
+      <c r="AIG17" s="53"/>
+      <c r="AIH17" s="53"/>
+      <c r="AII17" s="53"/>
+      <c r="AIJ17" s="53"/>
+      <c r="AIK17" s="53"/>
+      <c r="AIL17" s="53"/>
+      <c r="AIM17" s="53"/>
+      <c r="AIN17" s="53"/>
+      <c r="AIO17" s="53"/>
+      <c r="AIP17" s="53"/>
+      <c r="AIQ17" s="53"/>
+      <c r="AIR17" s="53"/>
+      <c r="AIS17" s="53"/>
+      <c r="AIT17" s="53"/>
+      <c r="AIU17" s="53"/>
+      <c r="AIV17" s="53"/>
+      <c r="AIW17" s="53"/>
+      <c r="AIX17" s="53"/>
+      <c r="AIY17" s="53"/>
+      <c r="AIZ17" s="53"/>
+      <c r="AJA17" s="53"/>
+      <c r="AJB17" s="53"/>
+      <c r="AJC17" s="53"/>
+      <c r="AJD17" s="53"/>
+      <c r="AJE17" s="53"/>
+      <c r="AJF17" s="53"/>
+      <c r="AJG17" s="53"/>
+      <c r="AJH17" s="53"/>
+      <c r="AJI17" s="53"/>
+      <c r="AJJ17" s="53"/>
+      <c r="AJK17" s="53"/>
+      <c r="AJL17" s="53"/>
+      <c r="AJM17" s="53"/>
+      <c r="AJN17" s="53"/>
+      <c r="AJO17" s="53"/>
+      <c r="AJP17" s="53"/>
+      <c r="AJQ17" s="53"/>
+      <c r="AJR17" s="53"/>
+      <c r="AJS17" s="53"/>
+      <c r="AJT17" s="53"/>
+      <c r="AJU17" s="53"/>
+      <c r="AJV17" s="53"/>
+      <c r="AJW17" s="53"/>
+      <c r="AJX17" s="53"/>
+      <c r="AJY17" s="53"/>
+      <c r="AJZ17" s="53"/>
+      <c r="AKA17" s="53"/>
+      <c r="AKB17" s="53"/>
+      <c r="AKC17" s="53"/>
+      <c r="AKD17" s="53"/>
+      <c r="AKE17" s="53"/>
+      <c r="AKF17" s="53"/>
+      <c r="AKG17" s="53"/>
+      <c r="AKH17" s="53"/>
+      <c r="AKI17" s="53"/>
+      <c r="AKJ17" s="53"/>
+      <c r="AKK17" s="53"/>
+      <c r="AKL17" s="53"/>
+      <c r="AKM17" s="53"/>
+      <c r="AKN17" s="53"/>
+      <c r="AKO17" s="53"/>
+      <c r="AKP17" s="53"/>
+      <c r="AKQ17" s="53"/>
+      <c r="AKR17" s="53"/>
+      <c r="AKS17" s="53"/>
+      <c r="AKT17" s="53"/>
+      <c r="AKU17" s="53"/>
+      <c r="AKV17" s="53"/>
+      <c r="AKW17" s="53"/>
+      <c r="AKX17" s="53"/>
+      <c r="AKY17" s="53"/>
+      <c r="AKZ17" s="53"/>
+      <c r="ALA17" s="53"/>
+      <c r="ALB17" s="53"/>
+      <c r="ALC17" s="53"/>
+      <c r="ALD17" s="53"/>
+      <c r="ALE17" s="53"/>
+      <c r="ALF17" s="53"/>
+      <c r="ALG17" s="53"/>
+      <c r="ALH17" s="53"/>
+      <c r="ALI17" s="53"/>
+      <c r="ALJ17" s="53"/>
+      <c r="ALK17" s="53"/>
+      <c r="ALL17" s="53"/>
+      <c r="ALM17" s="53"/>
+      <c r="ALN17" s="53"/>
+      <c r="ALO17" s="53"/>
+      <c r="ALP17" s="53"/>
+      <c r="ALQ17" s="53"/>
+      <c r="ALR17" s="53"/>
+      <c r="ALS17" s="53"/>
+      <c r="ALT17" s="53"/>
+      <c r="ALU17" s="53"/>
+      <c r="ALV17" s="53"/>
+      <c r="ALW17" s="53"/>
+      <c r="ALX17" s="53"/>
+      <c r="ALY17" s="53"/>
+      <c r="ALZ17" s="53"/>
+      <c r="AMA17" s="53"/>
+      <c r="AMB17" s="53"/>
+      <c r="AMC17" s="53"/>
+      <c r="AMD17" s="53"/>
+      <c r="AME17" s="53"/>
+      <c r="AMF17" s="53"/>
+      <c r="AMG17" s="53"/>
+      <c r="AMH17" s="53"/>
+      <c r="AMI17" s="53"/>
+      <c r="AMJ17" s="53"/>
+      <c r="AMK17" s="53"/>
+      <c r="AML17" s="53"/>
+      <c r="AMM17" s="53"/>
+      <c r="AMN17" s="53"/>
     </row>
-    <row r="18" customFormat="1" ht="28" customHeight="1" spans="1:1027">
+    <row r="18" customFormat="1" ht="28" customHeight="1" spans="1:1028">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -3716,14 +3762,14 @@
       <c r="N18" s="15"/>
       <c r="O18" s="33"/>
       <c r="P18" s="33"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="30"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="30"/>
-      <c r="U18" s="15"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="30"/>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
-      <c r="X18" s="5"/>
+      <c r="X18" s="15"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
@@ -4727,10 +4773,11 @@
       <c r="AMK18" s="5"/>
       <c r="AML18" s="5"/>
       <c r="AMM18" s="5"/>
+      <c r="AMN18" s="5"/>
     </row>
-    <row r="19" ht="23" customHeight="1" spans="1:25">
+    <row r="19" ht="23" customHeight="1" spans="1:26">
       <c r="A19" s="16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
@@ -4755,17 +4802,18 @@
       <c r="V19" s="17"/>
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
-      <c r="Y19" s="56"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="54"/>
     </row>
-    <row r="20" ht="15.75" spans="1:25">
+    <row r="20" spans="1:26">
       <c r="A20" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20" s="19">
         <v>0</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" s="19">
         <v>416</v>
@@ -4786,7 +4834,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K20" s="18">
         <v>24</v>
@@ -4798,47 +4846,48 @@
         <v>0.0003</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O20" s="34">
         <v>0.0005</v>
       </c>
       <c r="P20" s="34"/>
-      <c r="Q20" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="R20" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="S20" s="19">
+      <c r="Q20" s="34"/>
+      <c r="R20" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="S20" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="T20" s="19">
         <v>0</v>
       </c>
-      <c r="T20" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="U20" s="19">
+      <c r="U20" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="V20" s="19">
         <v>0.9837</v>
       </c>
-      <c r="V20" s="48">
+      <c r="W20" s="46">
         <v>0.972</v>
       </c>
-      <c r="W20" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="X20" s="49" t="s">
+      <c r="X20" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="Y20" s="44"/>
+      <c r="Y20" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z20" s="43"/>
     </row>
-    <row r="21" ht="15.75" spans="1:25">
+    <row r="21" spans="1:26">
       <c r="A21" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B21" s="10">
         <v>0</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" s="10">
         <v>416</v>
@@ -4859,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K21" s="9">
         <v>24</v>
@@ -4871,45 +4920,46 @@
         <v>0.0001</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O21" s="31">
         <v>0.0005</v>
       </c>
       <c r="P21" s="31"/>
-      <c r="Q21" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="R21" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="S21" s="10">
+      <c r="Q21" s="31"/>
+      <c r="R21" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="S21" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T21" s="10">
         <v>0</v>
       </c>
-      <c r="T21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U21" s="10">
+      <c r="U21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V21" s="10">
         <v>0.9846</v>
       </c>
-      <c r="V21" s="50">
+      <c r="W21" s="47">
         <v>0.973</v>
       </c>
-      <c r="W21" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="X21" s="44"/>
-      <c r="Y21" s="44"/>
+      <c r="X21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y21" s="43"/>
+      <c r="Z21" s="43"/>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:26">
       <c r="A22" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="21">
         <v>0</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D22" s="21">
         <v>416</v>
@@ -4930,7 +4980,7 @@
         <v>1</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K22" s="22">
         <v>24</v>
@@ -4942,49 +4992,50 @@
         <v>0.0003</v>
       </c>
       <c r="N22" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O22" s="36">
         <v>0.0005</v>
       </c>
       <c r="P22" s="36"/>
-      <c r="Q22" s="22" t="s">
-        <v>49</v>
-      </c>
+      <c r="Q22" s="36"/>
       <c r="R22" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S22" s="22">
+        <v>50</v>
+      </c>
+      <c r="S22" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="T22" s="22">
         <v>0</v>
       </c>
-      <c r="T22" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="U22" s="22">
+      <c r="U22" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="V22" s="22">
         <v>0.9846</v>
       </c>
-      <c r="V22" s="51">
+      <c r="W22" s="48">
         <v>0.974</v>
       </c>
-      <c r="W22" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="X22" s="44" t="s">
+      <c r="X22" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="Y22" s="44" t="s">
+      <c r="Y22" s="43" t="s">
         <v>58</v>
       </c>
+      <c r="Z22" s="43" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="23" ht="15.75" spans="1:25">
+    <row r="23" spans="1:26">
       <c r="A23" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="10">
         <v>0</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D23" s="10">
         <v>416</v>
@@ -5005,7 +5056,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K23" s="9">
         <v>24</v>
@@ -5017,45 +5068,46 @@
         <v>0.0001</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O23" s="31">
         <v>0.0005</v>
       </c>
       <c r="P23" s="31"/>
-      <c r="Q23" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="R23" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="S23" s="10">
+      <c r="Q23" s="31"/>
+      <c r="R23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T23" s="10">
         <v>0</v>
       </c>
-      <c r="T23" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U23" s="10">
+      <c r="U23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V23" s="10">
         <v>0.9861</v>
       </c>
-      <c r="V23" s="52">
+      <c r="W23" s="49">
         <v>0.971</v>
       </c>
-      <c r="W23" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="X23" s="44"/>
-      <c r="Y23" s="44"/>
+      <c r="X23" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y23" s="43"/>
+      <c r="Z23" s="43"/>
     </row>
-    <row r="24" ht="15.75" spans="1:25">
+    <row r="24" spans="1:26">
       <c r="A24" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" s="10">
         <v>0</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D24" s="10">
         <v>416</v>
@@ -5076,7 +5128,7 @@
         <v>1</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K24" s="9">
         <v>24</v>
@@ -5088,47 +5140,48 @@
         <v>0.0003</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="O24" s="31">
         <v>0.0005</v>
       </c>
       <c r="P24" s="31"/>
-      <c r="Q24" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="R24" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="S24" s="10">
+      <c r="Q24" s="31"/>
+      <c r="R24" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="T24" s="10">
         <v>0</v>
       </c>
-      <c r="T24" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="U24" s="10">
+      <c r="U24" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V24" s="10">
         <v>0.9856</v>
       </c>
-      <c r="V24" s="52">
+      <c r="W24" s="49">
         <v>0.97</v>
       </c>
-      <c r="W24" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="X24" s="44" t="s">
+      <c r="X24" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Y24" s="44"/>
+      <c r="Y24" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z24" s="43"/>
     </row>
-    <row r="25" s="4" customFormat="1" ht="15.75" spans="1:1027">
+    <row r="25" s="4" customFormat="1" ht="15.75" spans="1:1028">
       <c r="A25" s="22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B25" s="22">
         <v>0</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D25" s="23">
         <v>384</v>
@@ -5149,7 +5202,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K25" s="22">
         <v>24</v>
@@ -5161,38 +5214,38 @@
         <v>0.0003</v>
       </c>
       <c r="N25" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O25" s="36">
         <v>0.0005</v>
       </c>
       <c r="P25" s="36"/>
-      <c r="Q25" s="22" t="s">
-        <v>49</v>
-      </c>
+      <c r="Q25" s="36"/>
       <c r="R25" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S25" s="22">
+        <v>50</v>
+      </c>
+      <c r="S25" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="T25" s="22">
         <v>0</v>
       </c>
-      <c r="T25" s="22" t="s">
-        <v>36</v>
-      </c>
       <c r="U25" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="V25" s="51">
+        <v>37</v>
+      </c>
+      <c r="V25" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="W25" s="48">
         <v>0.976</v>
       </c>
-      <c r="W25" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="X25" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y25" s="53"/>
-      <c r="Z25" s="57"/>
+      <c r="X25" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y25" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z25" s="56"/>
       <c r="AA25" s="57"/>
       <c r="AB25" s="57"/>
       <c r="AC25" s="57"/>
@@ -6194,16 +6247,17 @@
       <c r="AMK25" s="57"/>
       <c r="AML25" s="57"/>
       <c r="AMM25" s="57"/>
+      <c r="AMN25" s="57"/>
     </row>
-    <row r="26" ht="15.75" spans="1:25">
+    <row r="26" spans="1:26">
       <c r="A26" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="21">
         <v>0</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D26" s="21">
         <v>416</v>
@@ -6224,7 +6278,7 @@
         <v>1</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K26" s="22">
         <v>24</v>
@@ -6236,47 +6290,48 @@
         <v>0.0003</v>
       </c>
       <c r="N26" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O26" s="36">
         <v>0.0005</v>
       </c>
       <c r="P26" s="36"/>
-      <c r="Q26" s="22" t="s">
-        <v>49</v>
-      </c>
+      <c r="Q26" s="36"/>
       <c r="R26" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S26" s="22">
+        <v>50</v>
+      </c>
+      <c r="S26" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="T26" s="22">
         <v>0</v>
       </c>
-      <c r="T26" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="U26" s="22">
+      <c r="U26" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="V26" s="22">
         <v>0.9918</v>
       </c>
-      <c r="V26" s="51">
+      <c r="W26" s="48">
         <v>0.976</v>
       </c>
-      <c r="W26" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="X26" s="44" t="s">
+      <c r="X26" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="Y26" s="44"/>
+      <c r="Y26" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z26" s="43"/>
     </row>
-    <row r="27" ht="15.75" spans="1:25">
+    <row r="27" spans="1:26">
       <c r="A27" s="25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B27" s="26">
         <v>0</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D27" s="26">
         <v>416</v>
@@ -6297,7 +6352,7 @@
         <v>1</v>
       </c>
       <c r="J27" s="28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K27" s="28">
         <v>24</v>
@@ -6309,47 +6364,48 @@
         <v>0.0003</v>
       </c>
       <c r="N27" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O27" s="37">
         <v>0.0005</v>
       </c>
       <c r="P27" s="37"/>
-      <c r="Q27" s="28" t="s">
-        <v>49</v>
-      </c>
+      <c r="Q27" s="37"/>
       <c r="R27" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="S27" s="28">
+        <v>50</v>
+      </c>
+      <c r="S27" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="T27" s="28">
         <v>0</v>
       </c>
-      <c r="T27" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="U27" s="28">
+      <c r="U27" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="V27" s="28">
         <v>0.9861</v>
       </c>
-      <c r="V27" s="54">
+      <c r="W27" s="50">
         <v>0.974</v>
       </c>
-      <c r="W27" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="X27" s="44" t="s">
+      <c r="X27" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="Y27" s="44"/>
+      <c r="Y27" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z27" s="43"/>
     </row>
-    <row r="28" ht="15.75" spans="1:25">
+    <row r="28" spans="1:26">
       <c r="A28" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28" s="21">
         <v>0</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D28" s="21">
         <v>416</v>
@@ -6370,7 +6426,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K28" s="22">
         <v>24</v>
@@ -6382,7 +6438,7 @@
         <v>0.0003</v>
       </c>
       <c r="N28" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O28" s="36">
         <v>0.0005</v>
@@ -6390,43 +6446,44 @@
       <c r="P28" s="38" t="b">
         <v>1</v>
       </c>
-      <c r="Q28" s="22" t="s">
-        <v>49</v>
-      </c>
+      <c r="Q28" s="36"/>
       <c r="R28" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S28" s="22">
+        <v>50</v>
+      </c>
+      <c r="S28" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="T28" s="22">
         <v>0</v>
       </c>
-      <c r="T28" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="U28" s="22">
+      <c r="U28" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="V28" s="22">
         <v>0.9861</v>
       </c>
-      <c r="V28" s="51">
+      <c r="W28" s="48">
         <v>0.976</v>
       </c>
-      <c r="W28" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="X28" s="44" t="s">
+      <c r="X28" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="Y28" s="44" t="s">
+      <c r="Y28" s="43" t="s">
         <v>73</v>
       </c>
+      <c r="Z28" s="43" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="29" ht="15.75" spans="1:25">
+    <row r="29" ht="15.75" spans="1:26">
       <c r="A29" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B29" s="21">
         <v>0</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D29" s="21">
         <v>416</v>
@@ -6447,7 +6504,7 @@
         <v>1</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K29" s="22">
         <v>24</v>
@@ -6459,50 +6516,177 @@
         <v>0.0003</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O29" s="36">
         <v>0.0005</v>
       </c>
       <c r="P29" s="36"/>
-      <c r="Q29" s="22" t="s">
-        <v>49</v>
-      </c>
+      <c r="Q29" s="36"/>
       <c r="R29" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="S29" s="22">
+        <v>50</v>
+      </c>
+      <c r="S29" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="T29" s="22">
         <v>0</v>
       </c>
-      <c r="T29" s="22" t="s">
+      <c r="U29" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="V29" s="22">
+        <v>0.9875</v>
+      </c>
+      <c r="W29" s="48">
+        <v>0.976</v>
+      </c>
+      <c r="X29" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y29" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z29" s="43"/>
+    </row>
+    <row r="30" ht="15.75" spans="1:26">
+      <c r="A30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="10">
+        <v>0</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="10">
+        <v>416</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="I30" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="9">
+        <v>24</v>
+      </c>
+      <c r="L30" s="9">
+        <v>45</v>
+      </c>
+      <c r="M30" s="31">
+        <v>0.0003</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O30" s="31">
+        <v>0.0005</v>
+      </c>
+      <c r="P30" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="S30" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="U29" s="22">
-        <v>0.9875</v>
-      </c>
-      <c r="V29" s="51">
-        <v>0.976</v>
-      </c>
-      <c r="W29" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="X29" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="Y29" s="44"/>
+      <c r="T30" s="10">
+        <v>0</v>
+      </c>
+      <c r="U30" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V30" s="10">
+        <v>0.9907</v>
+      </c>
+      <c r="W30" s="49">
+        <v>0.974</v>
+      </c>
+      <c r="X30" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y30" s="43" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z30" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:J1"/>
-    <mergeCell ref="K1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="A15:V15"/>
-    <mergeCell ref="A19:Y19"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="A15:W15"/>
+    <mergeCell ref="A19:Z19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5"/>
+  <cols>
+    <col min="1" max="1" width="62.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix some bugs when using selected_labels
</commit_message>
<xml_diff>
--- a/record_mxq.xlsx
+++ b/record_mxq.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="91">
   <si>
     <t>Model</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>观察曲线，加大batch_size、epoch</t>
+  </si>
+  <si>
+    <t>log-2019-12-17T18-24-58</t>
+  </si>
+  <si>
+    <t>重新训练带来微小提升</t>
   </si>
   <si>
     <t>Apple</t>
@@ -1722,7 +1728,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
@@ -3710,6 +3716,80 @@
         <v>82</v>
       </c>
     </row>
+    <row r="32" customFormat="1" ht="15.75" spans="1:26">
+      <c r="A32" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="21">
+        <v>0</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="21">
+        <v>416</v>
+      </c>
+      <c r="E32" s="21">
+        <v>0</v>
+      </c>
+      <c r="F32" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G32" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="H32" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="I32" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="22">
+        <v>24</v>
+      </c>
+      <c r="L32" s="22">
+        <v>30</v>
+      </c>
+      <c r="M32" s="38">
+        <v>0.0003</v>
+      </c>
+      <c r="N32" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="O32" s="38">
+        <v>0.0005</v>
+      </c>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="S32" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="T32" s="22">
+        <v>0</v>
+      </c>
+      <c r="U32" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="V32" s="22">
+        <v>0.987</v>
+      </c>
+      <c r="W32" s="50">
+        <v>0.976</v>
+      </c>
+      <c r="X32" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y32" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z32" s="45"/>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A1:B1"/>
@@ -3742,32 +3822,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add warmup RAdam res2net
</commit_message>
<xml_diff>
--- a/record_mxq.xlsx
+++ b/record_mxq.xlsx
@@ -296,9 +296,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
@@ -342,23 +342,23 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -371,7 +371,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -386,22 +386,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,8 +401,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -437,13 +431,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -461,7 +448,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -469,14 +471,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -490,13 +484,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="44">
     <fill>
@@ -585,13 +585,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,157 +753,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -944,6 +944,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -959,17 +974,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1000,26 +1009,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1028,142 +1028,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="39" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1243,9 +1243,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1730,8 +1727,8 @@
   <sheetPr/>
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="M8" workbookViewId="0">
+      <selection activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1770,44 +1767,44 @@
         <v>1</v>
       </c>
       <c r="D1" s="7"/>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="30" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="41" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="T1" s="41"/>
-      <c r="U1" s="42" t="s">
+      <c r="T1" s="40"/>
+      <c r="U1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="41" t="s">
+      <c r="V1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="43" t="s">
+      <c r="W1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="44" t="s">
+      <c r="X1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="53" t="s">
+      <c r="Y1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="54" t="s">
+      <c r="Z1" s="53" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1911,17 +1908,17 @@
       <c r="L3" s="9">
         <v>60</v>
       </c>
-      <c r="M3" s="33">
+      <c r="M3" s="32">
         <v>0.01</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="33">
+      <c r="O3" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
       <c r="R3" s="9" t="s">
         <v>35</v>
       </c>
@@ -1940,7 +1937,7 @@
       <c r="W3" s="9">
         <v>0.954</v>
       </c>
-      <c r="X3" s="45"/>
+      <c r="X3" s="44"/>
     </row>
     <row r="4" ht="22.5" customHeight="1" spans="1:24">
       <c r="A4" s="9" t="s">
@@ -1977,17 +1974,17 @@
       <c r="L4" s="9">
         <v>60</v>
       </c>
-      <c r="M4" s="33">
+      <c r="M4" s="32">
         <v>0.01</v>
       </c>
       <c r="N4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
       <c r="R4" s="9" t="s">
         <v>35</v>
       </c>
@@ -2006,7 +2003,7 @@
       <c r="W4" s="9">
         <v>0.946</v>
       </c>
-      <c r="X4" s="45"/>
+      <c r="X4" s="44"/>
     </row>
     <row r="5" ht="21.75" customHeight="1" spans="1:24">
       <c r="A5" s="9" t="s">
@@ -2043,17 +2040,17 @@
       <c r="L5" s="9">
         <v>60</v>
       </c>
-      <c r="M5" s="33">
+      <c r="M5" s="32">
         <v>0.01</v>
       </c>
       <c r="N5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
       <c r="R5" s="9" t="s">
         <v>35</v>
       </c>
@@ -2072,7 +2069,7 @@
       <c r="W5" s="9">
         <v>0.949</v>
       </c>
-      <c r="X5" s="45"/>
+      <c r="X5" s="44"/>
     </row>
     <row r="6" ht="18.75" customHeight="1" spans="1:24">
       <c r="A6" s="9" t="s">
@@ -2109,17 +2106,17 @@
       <c r="L6" s="9">
         <v>60</v>
       </c>
-      <c r="M6" s="33">
+      <c r="M6" s="32">
         <v>0.01</v>
       </c>
       <c r="N6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O6" s="33">
+      <c r="O6" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
       <c r="R6" s="9" t="s">
         <v>35</v>
       </c>
@@ -2138,7 +2135,7 @@
       <c r="W6" s="9">
         <v>0.952</v>
       </c>
-      <c r="X6" s="45"/>
+      <c r="X6" s="44"/>
     </row>
     <row r="7" ht="18.75" customHeight="1" spans="1:24">
       <c r="A7" s="9" t="s">
@@ -2175,17 +2172,17 @@
       <c r="L7" s="9">
         <v>60</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="32">
         <v>0.01</v>
       </c>
       <c r="N7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
       <c r="R7" s="9" t="s">
         <v>35</v>
       </c>
@@ -2204,7 +2201,7 @@
       <c r="W7" s="9">
         <v>0.958</v>
       </c>
-      <c r="X7" s="45"/>
+      <c r="X7" s="44"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:24">
       <c r="A8" s="9" t="s">
@@ -2241,17 +2238,17 @@
       <c r="L8" s="9">
         <v>60</v>
       </c>
-      <c r="M8" s="33">
+      <c r="M8" s="32">
         <v>0.01</v>
       </c>
       <c r="N8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="33">
+      <c r="O8" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
       <c r="R8" s="9" t="s">
         <v>35</v>
       </c>
@@ -2270,7 +2267,7 @@
       <c r="W8" s="9">
         <v>0.959</v>
       </c>
-      <c r="X8" s="45"/>
+      <c r="X8" s="44"/>
     </row>
     <row r="9" ht="17.25" customHeight="1" spans="1:24">
       <c r="A9" s="9" t="s">
@@ -2307,17 +2304,17 @@
       <c r="L9" s="9">
         <v>60</v>
       </c>
-      <c r="M9" s="33">
+      <c r="M9" s="32">
         <v>0.01</v>
       </c>
       <c r="N9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
       <c r="R9" s="9" t="s">
         <v>35</v>
       </c>
@@ -2336,7 +2333,7 @@
       <c r="W9" s="9">
         <v>0.961</v>
       </c>
-      <c r="X9" s="45"/>
+      <c r="X9" s="44"/>
     </row>
     <row r="10" ht="17.25" customHeight="1" spans="1:24">
       <c r="A10" s="9" t="s">
@@ -2373,17 +2370,17 @@
       <c r="L10" s="9">
         <v>50</v>
       </c>
-      <c r="M10" s="33">
+      <c r="M10" s="32">
         <v>0.01</v>
       </c>
       <c r="N10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="O10" s="33">
+      <c r="O10" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="33"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
       <c r="R10" s="9" t="s">
         <v>35</v>
       </c>
@@ -2402,7 +2399,7 @@
       <c r="W10" s="9">
         <v>0.964</v>
       </c>
-      <c r="X10" s="45"/>
+      <c r="X10" s="44"/>
     </row>
     <row r="11" ht="19.5" customHeight="1"/>
     <row r="12" ht="18" customHeight="1" spans="1:24">
@@ -2440,17 +2437,17 @@
       <c r="L12" s="9">
         <v>50</v>
       </c>
-      <c r="M12" s="33">
+      <c r="M12" s="32">
         <v>0.002</v>
       </c>
       <c r="N12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O12" s="33">
+      <c r="O12" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
       <c r="R12" s="10" t="s">
         <v>35</v>
       </c>
@@ -2469,9 +2466,9 @@
       <c r="W12" s="10">
         <v>0.964</v>
       </c>
-      <c r="X12" s="45"/>
+      <c r="X12" s="44"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" ht="15.75" spans="1:24">
       <c r="A13" s="9" t="s">
         <v>39</v>
       </c>
@@ -2506,17 +2503,17 @@
       <c r="L13" s="9">
         <v>60</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="32">
         <v>0.001</v>
       </c>
       <c r="N13" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="O13" s="33">
+      <c r="O13" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
       <c r="R13" s="10" t="s">
         <v>35</v>
       </c>
@@ -2535,7 +2532,7 @@
       <c r="W13" s="10">
         <v>0.955</v>
       </c>
-      <c r="X13" s="45"/>
+      <c r="X13" s="44"/>
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:24">
       <c r="A14" s="9" t="s">
@@ -2572,17 +2569,17 @@
       <c r="L14" s="9">
         <v>30</v>
       </c>
-      <c r="M14" s="33" t="s">
+      <c r="M14" s="32" t="s">
         <v>49</v>
       </c>
       <c r="N14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="33">
+      <c r="O14" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
       <c r="R14" s="10" t="s">
         <v>50</v>
       </c>
@@ -2601,7 +2598,7 @@
       <c r="W14" s="21">
         <v>0.971</v>
       </c>
-      <c r="X14" s="45"/>
+      <c r="X14" s="44"/>
     </row>
     <row r="15" ht="20.25" customHeight="1" spans="1:23">
       <c r="A15" s="11" t="s">
@@ -2665,17 +2662,17 @@
       <c r="L16" s="12">
         <v>30</v>
       </c>
-      <c r="M16" s="34" t="s">
+      <c r="M16" s="33" t="s">
         <v>49</v>
       </c>
       <c r="N16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="O16" s="34">
+      <c r="O16" s="33">
         <v>0.0005</v>
       </c>
-      <c r="P16" s="34"/>
-      <c r="Q16" s="34"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
       <c r="R16" s="13" t="s">
         <v>50</v>
       </c>
@@ -2691,10 +2688,10 @@
       <c r="V16" s="13">
         <v>0.9837</v>
       </c>
-      <c r="W16" s="46">
+      <c r="W16" s="45">
         <v>0.974</v>
       </c>
-      <c r="X16" s="45"/>
+      <c r="X16" s="44"/>
     </row>
     <row r="17" s="3" customFormat="1" ht="15.75" spans="1:26">
       <c r="A17" s="12" t="s">
@@ -2731,17 +2728,17 @@
       <c r="L17" s="12">
         <v>60</v>
       </c>
-      <c r="M17" s="34">
+      <c r="M17" s="33">
         <v>0.0003</v>
       </c>
       <c r="N17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="O17" s="34">
+      <c r="O17" s="33">
         <v>0.0005</v>
       </c>
-      <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
       <c r="R17" s="13" t="s">
         <v>50</v>
       </c>
@@ -2760,9 +2757,9 @@
       <c r="W17" s="13">
         <v>0.955</v>
       </c>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="55"/>
+      <c r="X17" s="46"/>
+      <c r="Y17" s="54"/>
+      <c r="Z17" s="54"/>
     </row>
     <row r="18" customFormat="1" ht="28" customHeight="1" spans="1:26">
       <c r="A18" s="14"/>
@@ -2774,18 +2771,18 @@
       <c r="G18" s="15"/>
       <c r="H18" s="15"/>
       <c r="I18" s="15"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="35"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="30"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="34"/>
       <c r="N18" s="15"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
       <c r="R18" s="15"/>
-      <c r="S18" s="31"/>
+      <c r="S18" s="30"/>
       <c r="T18" s="15"/>
-      <c r="U18" s="31"/>
+      <c r="U18" s="30"/>
       <c r="V18" s="15"/>
       <c r="W18" s="15"/>
       <c r="X18" s="15"/>
@@ -2820,9 +2817,9 @@
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
       <c r="Y19" s="17"/>
-      <c r="Z19" s="56"/>
+      <c r="Z19" s="55"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" ht="15.75" spans="1:26">
       <c r="A20" s="18" t="s">
         <v>39</v>
       </c>
@@ -2859,17 +2856,17 @@
       <c r="L20" s="18">
         <v>50</v>
       </c>
-      <c r="M20" s="36">
+      <c r="M20" s="35">
         <v>0.0003</v>
       </c>
       <c r="N20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="O20" s="36">
+      <c r="O20" s="35">
         <v>0.0005</v>
       </c>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="35"/>
       <c r="R20" s="19" t="s">
         <v>50</v>
       </c>
@@ -2885,18 +2882,18 @@
       <c r="V20" s="19">
         <v>0.9837</v>
       </c>
-      <c r="W20" s="48">
+      <c r="W20" s="47">
         <v>0.972</v>
       </c>
       <c r="X20" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="Y20" s="57" t="s">
+      <c r="Y20" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="Z20" s="45"/>
+      <c r="Z20" s="44"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" ht="15.75" spans="1:26">
       <c r="A21" s="9" t="s">
         <v>39</v>
       </c>
@@ -2933,17 +2930,17 @@
       <c r="L21" s="9">
         <v>50</v>
       </c>
-      <c r="M21" s="37">
+      <c r="M21" s="36">
         <v>0.0001</v>
       </c>
       <c r="N21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O21" s="33">
+      <c r="O21" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
       <c r="R21" s="10" t="s">
         <v>50</v>
       </c>
@@ -2959,16 +2956,16 @@
       <c r="V21" s="10">
         <v>0.9846</v>
       </c>
-      <c r="W21" s="49">
+      <c r="W21" s="48">
         <v>0.973</v>
       </c>
       <c r="X21" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="Y21" s="45"/>
-      <c r="Z21" s="45"/>
+      <c r="Y21" s="44"/>
+      <c r="Z21" s="44"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" ht="15.75" spans="1:26">
       <c r="A22" s="20" t="s">
         <v>39</v>
       </c>
@@ -3005,17 +3002,17 @@
       <c r="L22" s="22">
         <v>40</v>
       </c>
-      <c r="M22" s="38">
+      <c r="M22" s="37">
         <v>0.0003</v>
       </c>
       <c r="N22" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="O22" s="38">
+      <c r="O22" s="37">
         <v>0.0005</v>
       </c>
-      <c r="P22" s="38"/>
-      <c r="Q22" s="38"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
       <c r="R22" s="22" t="s">
         <v>50</v>
       </c>
@@ -3031,20 +3028,20 @@
       <c r="V22" s="22">
         <v>0.9846</v>
       </c>
-      <c r="W22" s="50">
+      <c r="W22" s="49">
         <v>0.974</v>
       </c>
       <c r="X22" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="Y22" s="45" t="s">
+      <c r="Y22" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="Z22" s="45" t="s">
+      <c r="Z22" s="44" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" ht="15.75" spans="1:26">
       <c r="A23" s="9" t="s">
         <v>39</v>
       </c>
@@ -3081,17 +3078,17 @@
       <c r="L23" s="9">
         <v>45</v>
       </c>
-      <c r="M23" s="33">
+      <c r="M23" s="32">
         <v>0.0001</v>
       </c>
       <c r="N23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O23" s="33">
+      <c r="O23" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
       <c r="R23" s="10" t="s">
         <v>50</v>
       </c>
@@ -3107,16 +3104,16 @@
       <c r="V23" s="10">
         <v>0.9861</v>
       </c>
-      <c r="W23" s="51">
+      <c r="W23" s="50">
         <v>0.971</v>
       </c>
       <c r="X23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="45"/>
+      <c r="Y23" s="44"/>
+      <c r="Z23" s="44"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" ht="15.75" spans="1:26">
       <c r="A24" s="9" t="s">
         <v>39</v>
       </c>
@@ -3153,17 +3150,17 @@
       <c r="L24" s="9">
         <v>40</v>
       </c>
-      <c r="M24" s="33">
+      <c r="M24" s="32">
         <v>0.0003</v>
       </c>
       <c r="N24" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="O24" s="33">
+      <c r="O24" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
       <c r="R24" s="10" t="s">
         <v>50</v>
       </c>
@@ -3179,16 +3176,16 @@
       <c r="V24" s="10">
         <v>0.9856</v>
       </c>
-      <c r="W24" s="51">
+      <c r="W24" s="50">
         <v>0.97</v>
       </c>
       <c r="X24" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Y24" s="45" t="s">
+      <c r="Y24" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="Z24" s="45"/>
+      <c r="Z24" s="44"/>
     </row>
     <row r="25" s="4" customFormat="1" ht="15.75" spans="1:26">
       <c r="A25" s="22" t="s">
@@ -3227,17 +3224,17 @@
       <c r="L25" s="22">
         <v>40</v>
       </c>
-      <c r="M25" s="38">
+      <c r="M25" s="37">
         <v>0.0003</v>
       </c>
       <c r="N25" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="O25" s="38">
+      <c r="O25" s="37">
         <v>0.0005</v>
       </c>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
       <c r="R25" s="22" t="s">
         <v>50</v>
       </c>
@@ -3253,18 +3250,18 @@
       <c r="V25" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="W25" s="50">
+      <c r="W25" s="49">
         <v>0.976</v>
       </c>
       <c r="X25" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="Y25" s="58" t="s">
+      <c r="Y25" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="Z25" s="58"/>
+      <c r="Z25" s="57"/>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" ht="15.75" spans="1:26">
       <c r="A26" s="20" t="s">
         <v>39</v>
       </c>
@@ -3301,17 +3298,17 @@
       <c r="L26" s="22">
         <v>40</v>
       </c>
-      <c r="M26" s="38">
+      <c r="M26" s="37">
         <v>0.0003</v>
       </c>
       <c r="N26" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="O26" s="38">
+      <c r="O26" s="37">
         <v>0.0005</v>
       </c>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
       <c r="R26" s="22" t="s">
         <v>50</v>
       </c>
@@ -3327,18 +3324,18 @@
       <c r="V26" s="22">
         <v>0.9918</v>
       </c>
-      <c r="W26" s="50">
+      <c r="W26" s="49">
         <v>0.976</v>
       </c>
       <c r="X26" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="Y26" s="45" t="s">
+      <c r="Y26" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="Z26" s="45"/>
+      <c r="Z26" s="44"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" ht="15.75" spans="1:26">
       <c r="A27" s="25" t="s">
         <v>69</v>
       </c>
@@ -3357,62 +3354,62 @@
       <c r="F27" s="26">
         <v>0.2</v>
       </c>
-      <c r="G27" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="H27" s="29">
+      <c r="G27" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="28">
         <v>0.25</v>
       </c>
-      <c r="I27" s="29" t="b">
+      <c r="I27" s="28" t="b">
         <v>1</v>
       </c>
-      <c r="J27" s="29" t="s">
+      <c r="J27" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="K27" s="29">
+      <c r="K27" s="28">
         <v>24</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="28">
         <v>40</v>
       </c>
-      <c r="M27" s="39">
+      <c r="M27" s="38">
         <v>0.0003</v>
       </c>
-      <c r="N27" s="29" t="s">
+      <c r="N27" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="O27" s="39">
+      <c r="O27" s="38">
         <v>0.0005</v>
       </c>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="39"/>
-      <c r="R27" s="29" t="s">
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="S27" s="29" t="s">
+      <c r="S27" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="T27" s="29">
-        <v>0</v>
-      </c>
-      <c r="U27" s="29" t="s">
+      <c r="T27" s="28">
+        <v>0</v>
+      </c>
+      <c r="U27" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="V27" s="29">
+      <c r="V27" s="28">
         <v>0.9861</v>
       </c>
-      <c r="W27" s="52">
+      <c r="W27" s="51">
         <v>0.974</v>
       </c>
-      <c r="X27" s="29" t="s">
+      <c r="X27" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="Y27" s="45" t="s">
+      <c r="Y27" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="Z27" s="45"/>
+      <c r="Z27" s="44"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" ht="15.75" spans="1:26">
       <c r="A28" s="20" t="s">
         <v>39</v>
       </c>
@@ -3449,19 +3446,19 @@
       <c r="L28" s="22">
         <v>40</v>
       </c>
-      <c r="M28" s="38">
+      <c r="M28" s="37">
         <v>0.0003</v>
       </c>
       <c r="N28" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="O28" s="38">
+      <c r="O28" s="37">
         <v>0.0005</v>
       </c>
-      <c r="P28" s="40" t="b">
+      <c r="P28" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="Q28" s="38"/>
+      <c r="Q28" s="37"/>
       <c r="R28" s="22" t="s">
         <v>50</v>
       </c>
@@ -3477,16 +3474,16 @@
       <c r="V28" s="22">
         <v>0.9861</v>
       </c>
-      <c r="W28" s="50">
+      <c r="W28" s="49">
         <v>0.976</v>
       </c>
       <c r="X28" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="Y28" s="45" t="s">
+      <c r="Y28" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="Z28" s="45" t="s">
+      <c r="Z28" s="44" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3524,20 +3521,20 @@
       <c r="K29" s="22">
         <v>24</v>
       </c>
-      <c r="L29" s="32">
+      <c r="L29" s="31">
         <v>30</v>
       </c>
-      <c r="M29" s="38">
+      <c r="M29" s="37">
         <v>0.0003</v>
       </c>
       <c r="N29" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="O29" s="38">
+      <c r="O29" s="37">
         <v>0.0005</v>
       </c>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="38"/>
+      <c r="P29" s="37"/>
+      <c r="Q29" s="37"/>
       <c r="R29" s="22" t="s">
         <v>50</v>
       </c>
@@ -3553,16 +3550,16 @@
       <c r="V29" s="22">
         <v>0.9875</v>
       </c>
-      <c r="W29" s="50">
+      <c r="W29" s="49">
         <v>0.976</v>
       </c>
       <c r="X29" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="Y29" s="45" t="s">
+      <c r="Y29" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="Z29" s="45"/>
+      <c r="Z29" s="44"/>
     </row>
     <row r="30" ht="15.75" spans="1:26">
       <c r="A30" s="9" t="s">
@@ -3601,19 +3598,19 @@
       <c r="L30" s="9">
         <v>45</v>
       </c>
-      <c r="M30" s="33">
+      <c r="M30" s="32">
         <v>0.0003</v>
       </c>
       <c r="N30" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O30" s="33">
+      <c r="O30" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P30" s="33" t="b">
+      <c r="P30" s="32" t="b">
         <v>1</v>
       </c>
-      <c r="Q30" s="33"/>
+      <c r="Q30" s="32"/>
       <c r="R30" s="10" t="s">
         <v>50</v>
       </c>
@@ -3629,43 +3626,43 @@
       <c r="V30" s="10">
         <v>0.9907</v>
       </c>
-      <c r="W30" s="51">
+      <c r="W30" s="50">
         <v>0.974</v>
       </c>
       <c r="X30" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="Y30" s="45" t="s">
+      <c r="Y30" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="Z30" s="45"/>
+      <c r="Z30" s="44"/>
     </row>
     <row r="31" ht="15.75" spans="1:26">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="27">
-        <v>0</v>
-      </c>
-      <c r="C31" s="27" t="s">
+      <c r="B31" s="10">
+        <v>0</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="10">
         <v>416</v>
       </c>
-      <c r="E31" s="27">
-        <v>0</v>
-      </c>
-      <c r="F31" s="27">
+      <c r="E31" s="10">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
         <v>0.2</v>
       </c>
-      <c r="G31" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="H31" s="27">
+      <c r="G31" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H31" s="10">
         <v>0.25</v>
       </c>
-      <c r="I31" s="27" t="b">
+      <c r="I31" s="10" t="b">
         <v>1</v>
       </c>
       <c r="J31" s="9" t="s">
@@ -3674,20 +3671,20 @@
       <c r="K31" s="9">
         <v>22</v>
       </c>
-      <c r="L31" s="27">
+      <c r="L31" s="10">
         <v>30</v>
       </c>
-      <c r="M31" s="33">
+      <c r="M31" s="32">
         <v>0.0003</v>
       </c>
       <c r="N31" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="O31" s="33">
+      <c r="O31" s="32">
         <v>0.0005</v>
       </c>
-      <c r="P31" s="27"/>
-      <c r="Q31" s="27"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
       <c r="R31" s="10" t="s">
         <v>50</v>
       </c>
@@ -3700,19 +3697,19 @@
       <c r="U31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="V31" s="27">
+      <c r="V31" s="10">
         <v>0.9822</v>
       </c>
-      <c r="W31" s="27">
+      <c r="W31" s="10">
         <v>0.969</v>
       </c>
-      <c r="X31" s="27" t="s">
+      <c r="X31" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="Y31" s="27" t="s">
+      <c r="Y31" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="Z31" s="27" t="s">
+      <c r="Z31" s="10" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3753,17 +3750,17 @@
       <c r="L32" s="22">
         <v>30</v>
       </c>
-      <c r="M32" s="38">
+      <c r="M32" s="37">
         <v>0.0003</v>
       </c>
       <c r="N32" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="O32" s="38">
+      <c r="O32" s="37">
         <v>0.0005</v>
       </c>
-      <c r="P32" s="38"/>
-      <c r="Q32" s="38"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="37"/>
       <c r="R32" s="22" t="s">
         <v>50</v>
       </c>
@@ -3779,16 +3776,16 @@
       <c r="V32" s="22">
         <v>0.987</v>
       </c>
-      <c r="W32" s="50">
-        <v>0.976</v>
+      <c r="W32" s="49">
+        <v>0.977</v>
       </c>
       <c r="X32" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="Y32" s="45" t="s">
+      <c r="Y32" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="Z32" s="45"/>
+      <c r="Z32" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
add val_official, saving dataset split file
</commit_message>
<xml_diff>
--- a/record_mxq.xlsx
+++ b/record_mxq.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="93">
   <si>
     <t>Model</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>重新训练带来微小提升</t>
+  </si>
+  <si>
+    <t>log-2019-12-20T08-42-53</t>
+  </si>
+  <si>
+    <t>去除权重衰减</t>
   </si>
   <si>
     <t>Apple</t>
@@ -296,10 +302,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -342,71 +348,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -418,59 +370,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,11 +394,117 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -573,6 +579,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -585,19 +597,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,151 +693,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -926,24 +938,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -955,6 +949,30 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -977,8 +995,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1009,17 +1027,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1028,142 +1040,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1299,7 +1311,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1311,7 +1326,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1320,10 +1335,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1725,10 +1740,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="M8" workbookViewId="0">
-      <selection activeCell="W33" sqref="W33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1801,10 +1816,10 @@
       <c r="X1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="52" t="s">
+      <c r="Y1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="Z1" s="53" t="s">
+      <c r="Z1" s="54" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2595,7 +2610,7 @@
       <c r="V14" s="10">
         <v>0.9827</v>
       </c>
-      <c r="W14" s="21">
+      <c r="W14" s="45">
         <v>0.971</v>
       </c>
       <c r="X14" s="44"/>
@@ -2688,7 +2703,7 @@
       <c r="V16" s="13">
         <v>0.9837</v>
       </c>
-      <c r="W16" s="45">
+      <c r="W16" s="46">
         <v>0.974</v>
       </c>
       <c r="X16" s="44"/>
@@ -2757,9 +2772,9 @@
       <c r="W17" s="13">
         <v>0.955</v>
       </c>
-      <c r="X17" s="46"/>
-      <c r="Y17" s="54"/>
-      <c r="Z17" s="54"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="55"/>
+      <c r="Z17" s="55"/>
     </row>
     <row r="18" customFormat="1" ht="28" customHeight="1" spans="1:26">
       <c r="A18" s="14"/>
@@ -2817,7 +2832,7 @@
       <c r="W19" s="17"/>
       <c r="X19" s="17"/>
       <c r="Y19" s="17"/>
-      <c r="Z19" s="55"/>
+      <c r="Z19" s="56"/>
     </row>
     <row r="20" ht="15.75" spans="1:26">
       <c r="A20" s="18" t="s">
@@ -2882,13 +2897,13 @@
       <c r="V20" s="19">
         <v>0.9837</v>
       </c>
-      <c r="W20" s="47">
+      <c r="W20" s="48">
         <v>0.972</v>
       </c>
       <c r="X20" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="Y20" s="56" t="s">
+      <c r="Y20" s="57" t="s">
         <v>55</v>
       </c>
       <c r="Z20" s="44"/>
@@ -2956,7 +2971,7 @@
       <c r="V21" s="10">
         <v>0.9846</v>
       </c>
-      <c r="W21" s="48">
+      <c r="W21" s="49">
         <v>0.973</v>
       </c>
       <c r="X21" s="10" t="s">
@@ -3028,7 +3043,7 @@
       <c r="V22" s="22">
         <v>0.9846</v>
       </c>
-      <c r="W22" s="49">
+      <c r="W22" s="50">
         <v>0.974</v>
       </c>
       <c r="X22" s="22" t="s">
@@ -3104,7 +3119,7 @@
       <c r="V23" s="10">
         <v>0.9861</v>
       </c>
-      <c r="W23" s="50">
+      <c r="W23" s="51">
         <v>0.971</v>
       </c>
       <c r="X23" s="10" t="s">
@@ -3176,7 +3191,7 @@
       <c r="V24" s="10">
         <v>0.9856</v>
       </c>
-      <c r="W24" s="50">
+      <c r="W24" s="51">
         <v>0.97</v>
       </c>
       <c r="X24" s="10" t="s">
@@ -3250,16 +3265,16 @@
       <c r="V25" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="W25" s="49">
+      <c r="W25" s="50">
         <v>0.976</v>
       </c>
       <c r="X25" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="Y25" s="57" t="s">
+      <c r="Y25" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="Z25" s="57"/>
+      <c r="Z25" s="58"/>
     </row>
     <row r="26" ht="15.75" spans="1:26">
       <c r="A26" s="20" t="s">
@@ -3324,7 +3339,7 @@
       <c r="V26" s="22">
         <v>0.9918</v>
       </c>
-      <c r="W26" s="49">
+      <c r="W26" s="50">
         <v>0.976</v>
       </c>
       <c r="X26" s="22" t="s">
@@ -3398,7 +3413,7 @@
       <c r="V27" s="28">
         <v>0.9861</v>
       </c>
-      <c r="W27" s="51">
+      <c r="W27" s="52">
         <v>0.974</v>
       </c>
       <c r="X27" s="28" t="s">
@@ -3474,7 +3489,7 @@
       <c r="V28" s="22">
         <v>0.9861</v>
       </c>
-      <c r="W28" s="49">
+      <c r="W28" s="50">
         <v>0.976</v>
       </c>
       <c r="X28" s="22" t="s">
@@ -3550,7 +3565,7 @@
       <c r="V29" s="22">
         <v>0.9875</v>
       </c>
-      <c r="W29" s="49">
+      <c r="W29" s="50">
         <v>0.976</v>
       </c>
       <c r="X29" s="22" t="s">
@@ -3626,7 +3641,7 @@
       <c r="V30" s="10">
         <v>0.9907</v>
       </c>
-      <c r="W30" s="50">
+      <c r="W30" s="51">
         <v>0.974</v>
       </c>
       <c r="X30" s="10" t="s">
@@ -3776,7 +3791,7 @@
       <c r="V32" s="22">
         <v>0.987</v>
       </c>
-      <c r="W32" s="49">
+      <c r="W32" s="50">
         <v>0.977</v>
       </c>
       <c r="X32" s="22" t="s">
@@ -3786,6 +3801,80 @@
         <v>84</v>
       </c>
       <c r="Z32" s="44"/>
+    </row>
+    <row r="33" customFormat="1" ht="15.75" spans="1:26">
+      <c r="A33" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="21">
+        <v>0</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="21">
+        <v>416</v>
+      </c>
+      <c r="E33" s="21">
+        <v>0</v>
+      </c>
+      <c r="F33" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G33" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="H33" s="22">
+        <v>0.25</v>
+      </c>
+      <c r="I33" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="22">
+        <v>24</v>
+      </c>
+      <c r="L33" s="22">
+        <v>30</v>
+      </c>
+      <c r="M33" s="37">
+        <v>0.0003</v>
+      </c>
+      <c r="N33" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="O33" s="37">
+        <v>0</v>
+      </c>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="37"/>
+      <c r="R33" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="S33" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="T33" s="22">
+        <v>0</v>
+      </c>
+      <c r="U33" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="V33" s="22">
+        <v>0.9875</v>
+      </c>
+      <c r="W33" s="50">
+        <v>0.978</v>
+      </c>
+      <c r="X33" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y33" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z33" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3819,32 +3908,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>